<commit_message>
2025-01-23 @ 08:46 - v5.N.3.xlsb - AUCUN CHANGEMENT DE CODE
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_File_Usage.xlsx
+++ b/DataFiles/GCF_File_Usage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79261281-3659-4A4D-93F6-D2EC56B7BCCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBCCA0AB-2A59-418D-B641-E78E5A54B97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C6563B4-B351-4CD7-B6BC-9B6B7E0B5346}"/>
   </bookViews>
@@ -484,7 +484,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B3F5A5B-0475-4A13-A512-AE71167667D2}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
@@ -685,6 +685,100 @@
         <v>3586</v>
       </c>
     </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>45679.715011574073</v>
+      </c>
+      <c r="B5" s="3">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3">
+        <v>187</v>
+      </c>
+      <c r="E5" s="3">
+        <v>364</v>
+      </c>
+      <c r="F5" s="3">
+        <v>340</v>
+      </c>
+      <c r="G5" s="3">
+        <v>384</v>
+      </c>
+      <c r="H5" s="3">
+        <v>2664</v>
+      </c>
+      <c r="I5" s="3">
+        <v>384</v>
+      </c>
+      <c r="J5" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K5" s="3">
+        <v>119</v>
+      </c>
+      <c r="L5" s="3">
+        <v>304</v>
+      </c>
+      <c r="M5" s="3">
+        <v>30</v>
+      </c>
+      <c r="N5" s="3">
+        <v>2864</v>
+      </c>
+      <c r="O5" s="3">
+        <v>3586</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>45680.001215277778</v>
+      </c>
+      <c r="B6" s="3">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3">
+        <v>187</v>
+      </c>
+      <c r="E6" s="3">
+        <v>364</v>
+      </c>
+      <c r="F6" s="3">
+        <v>340</v>
+      </c>
+      <c r="G6" s="3">
+        <v>384</v>
+      </c>
+      <c r="H6" s="3">
+        <v>2664</v>
+      </c>
+      <c r="I6" s="3">
+        <v>384</v>
+      </c>
+      <c r="J6" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K6" s="3">
+        <v>119</v>
+      </c>
+      <c r="L6" s="3">
+        <v>304</v>
+      </c>
+      <c r="M6" s="3">
+        <v>30</v>
+      </c>
+      <c r="N6" s="3">
+        <v>2864</v>
+      </c>
+      <c r="O6" s="3">
+        <v>3606</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2025-01-25 @ 14:35 - v5.N.3.xlsb - 25 935 lignes - Compile OK
* modAppli_Utils.bas
   - Ajuster le formatage de la feuille FAC_Détails après l'importation
* modFAC_Finale.bas
   - Dans 'FAC_Finale_Add_Invoice_Details_to_DB' ajouter la colonne TimeStamp
   - Dans 'FAC_Finale_Add_Invoice_Details_Locally' ajouter la colonne G (TimeStamp)
* modFunctions.bas
   - Éliminer du code mort
   - Changer l'appel au AF ('Fn_Get_TEC_Total_Invoice_AF'), pour tenir compte de la nouvelle colonne insérée en G
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_File_Usage.xlsx
+++ b/DataFiles/GCF_File_Usage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBCCA0AB-2A59-418D-B641-E78E5A54B97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03A5865-101D-4171-A646-6F03CD2129CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C6563B4-B351-4CD7-B6BC-9B6B7E0B5346}"/>
   </bookViews>
@@ -484,7 +484,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B3F5A5B-0475-4A13-A512-AE71167667D2}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
@@ -779,6 +779,53 @@
         <v>3606</v>
       </c>
     </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>45681.978125000001</v>
+      </c>
+      <c r="B7" s="3">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3">
+        <v>188</v>
+      </c>
+      <c r="E7" s="3">
+        <v>368</v>
+      </c>
+      <c r="F7" s="3">
+        <v>344</v>
+      </c>
+      <c r="G7" s="3">
+        <v>384</v>
+      </c>
+      <c r="H7" s="3">
+        <v>2664</v>
+      </c>
+      <c r="I7" s="3">
+        <v>384</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K7" s="3">
+        <v>119</v>
+      </c>
+      <c r="L7" s="3">
+        <v>304</v>
+      </c>
+      <c r="M7" s="3">
+        <v>30</v>
+      </c>
+      <c r="N7" s="3">
+        <v>2884</v>
+      </c>
+      <c r="O7" s="3">
+        <v>3651</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2025-02-03 @ 10:01 - v5.O.1.xlsb - 27 179 lignes - Compile OK
Pour tous les commentaires des logs, remplacer les '*' par des des '-'
Changer la référence de Now() @ Date si les heures, minutes et secondes ne sont pas souhaitables
* modGL_EJ.bas
- Après avoir observé de grandes lenteurs dans 'GL_Trans_Add_Record_Locally' j'ai ajouté des entrées au log pour analyse future
* modLog_Analysis.bas
- Travail pour l'exportation efficace des fichiers Logs dans le fichier central 'GCF_Logs_Data.xlsb' des Logs.
- Changer l'approche pour écrire dans le classeur 'GCF_Logs_Data.xlsb', ne plus utiliser ADO
* wshFAC_Historique.doccls
- Finaliser le traitement adéquat du clic droit dans la plage des factures
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_File_Usage.xlsx
+++ b/DataFiles/GCF_File_Usage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC4C9B9-C570-452F-8309-0440987E84A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E640DB-C45B-47DE-885D-25E7D51987E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C6563B4-B351-4CD7-B6BC-9B6B7E0B5346}"/>
   </bookViews>
@@ -484,7 +484,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B3F5A5B-0475-4A13-A512-AE71167667D2}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
@@ -1860,6 +1860,100 @@
         <v>3786</v>
       </c>
     </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>45690.329386574071</v>
+      </c>
+      <c r="B30" s="3">
+        <v>8</v>
+      </c>
+      <c r="C30" s="3">
+        <v>6</v>
+      </c>
+      <c r="D30" s="3">
+        <v>193</v>
+      </c>
+      <c r="E30" s="3">
+        <v>380</v>
+      </c>
+      <c r="F30" s="3">
+        <v>356</v>
+      </c>
+      <c r="G30" s="3">
+        <v>384</v>
+      </c>
+      <c r="H30" s="3">
+        <v>2664</v>
+      </c>
+      <c r="I30" s="3">
+        <v>384</v>
+      </c>
+      <c r="J30" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K30" s="3">
+        <v>119</v>
+      </c>
+      <c r="L30" s="3">
+        <v>304</v>
+      </c>
+      <c r="M30" s="3">
+        <v>30</v>
+      </c>
+      <c r="N30" s="3">
+        <v>2949</v>
+      </c>
+      <c r="O30" s="3">
+        <v>3791</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>45690.951608796298</v>
+      </c>
+      <c r="B31" s="3">
+        <v>8</v>
+      </c>
+      <c r="C31" s="3">
+        <v>6</v>
+      </c>
+      <c r="D31" s="3">
+        <v>193</v>
+      </c>
+      <c r="E31" s="3">
+        <v>380</v>
+      </c>
+      <c r="F31" s="3">
+        <v>356</v>
+      </c>
+      <c r="G31" s="3">
+        <v>384</v>
+      </c>
+      <c r="H31" s="3">
+        <v>2664</v>
+      </c>
+      <c r="I31" s="3">
+        <v>384</v>
+      </c>
+      <c r="J31" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K31" s="3">
+        <v>119</v>
+      </c>
+      <c r="L31" s="3">
+        <v>304</v>
+      </c>
+      <c r="M31" s="3">
+        <v>30</v>
+      </c>
+      <c r="N31" s="3">
+        <v>2977</v>
+      </c>
+      <c r="O31" s="3">
+        <v>3796</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2025-02-07 @ 07:27 - v5.P.0.xlsb - 28 189 lignes - Compile OK
Déplacer la déclaration de startTime au début du module (Globale) et modifier tous les appels à Log_Record, pour enlever Dim startTime as Double:
* modAppli_Utils.bas
- Modifier la vérification du Plan Comptable, en fonction du nouveau rôle du type de compte (pour états financiers)
* modFunctions.bas
- Modification de la fonction qui récupère les secondes (importation du log) puisque certains nombres arrivent avec un '.' comme séparateur décimal ??
* modGL_PrepEF.bas
- Nouveau module pour la production des états financiers (1 117 lignes)
* wshCAR_Liste_Agée.doccls
- Ajouter l'importation des 2 tables liées aux encaissements (Détails & Entête)
* wshGL_PrepEF.doccls
- Mise au point de la préparation des états financiers
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_File_Usage.xlsx
+++ b/DataFiles/GCF_File_Usage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E640DB-C45B-47DE-885D-25E7D51987E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2599963F-8F6D-4795-B357-78DD621EFD2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C6563B4-B351-4CD7-B6BC-9B6B7E0B5346}"/>
   </bookViews>
@@ -484,7 +484,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B3F5A5B-0475-4A13-A512-AE71167667D2}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
@@ -1954,6 +1954,288 @@
         <v>3796</v>
       </c>
     </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>45693.18645833333</v>
+      </c>
+      <c r="B32" s="3">
+        <v>8</v>
+      </c>
+      <c r="C32" s="3">
+        <v>6</v>
+      </c>
+      <c r="D32" s="3">
+        <v>195</v>
+      </c>
+      <c r="E32" s="3">
+        <v>380</v>
+      </c>
+      <c r="F32" s="3">
+        <v>356</v>
+      </c>
+      <c r="G32" s="3">
+        <v>384</v>
+      </c>
+      <c r="H32" s="3">
+        <v>2664</v>
+      </c>
+      <c r="I32" s="3">
+        <v>384</v>
+      </c>
+      <c r="J32" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K32" s="3">
+        <v>119</v>
+      </c>
+      <c r="L32" s="3">
+        <v>304</v>
+      </c>
+      <c r="M32" s="3">
+        <v>30</v>
+      </c>
+      <c r="N32" s="3">
+        <v>2985</v>
+      </c>
+      <c r="O32" s="3">
+        <v>3873</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>45693.191284722219</v>
+      </c>
+      <c r="B33" s="3">
+        <v>8</v>
+      </c>
+      <c r="C33" s="3">
+        <v>6</v>
+      </c>
+      <c r="D33" s="3">
+        <v>195</v>
+      </c>
+      <c r="E33" s="3">
+        <v>380</v>
+      </c>
+      <c r="F33" s="3">
+        <v>356</v>
+      </c>
+      <c r="G33" s="3">
+        <v>384</v>
+      </c>
+      <c r="H33" s="3">
+        <v>2664</v>
+      </c>
+      <c r="I33" s="3">
+        <v>384</v>
+      </c>
+      <c r="J33" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K33" s="3">
+        <v>119</v>
+      </c>
+      <c r="L33" s="3">
+        <v>304</v>
+      </c>
+      <c r="M33" s="3">
+        <v>30</v>
+      </c>
+      <c r="N33" s="3">
+        <v>2985</v>
+      </c>
+      <c r="O33" s="3">
+        <v>3873</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>45694.214224537034</v>
+      </c>
+      <c r="B34" s="3">
+        <v>8</v>
+      </c>
+      <c r="C34" s="3">
+        <v>6</v>
+      </c>
+      <c r="D34" s="3">
+        <v>196</v>
+      </c>
+      <c r="E34" s="3">
+        <v>381</v>
+      </c>
+      <c r="F34" s="3">
+        <v>357</v>
+      </c>
+      <c r="G34" s="3">
+        <v>384</v>
+      </c>
+      <c r="H34" s="3">
+        <v>2664</v>
+      </c>
+      <c r="I34" s="3">
+        <v>384</v>
+      </c>
+      <c r="J34" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K34" s="3">
+        <v>119</v>
+      </c>
+      <c r="L34" s="3">
+        <v>304</v>
+      </c>
+      <c r="M34" s="3">
+        <v>30</v>
+      </c>
+      <c r="N34" s="3">
+        <v>2993</v>
+      </c>
+      <c r="O34" s="3">
+        <v>3903</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>45694.21837962963</v>
+      </c>
+      <c r="B35" s="3">
+        <v>8</v>
+      </c>
+      <c r="C35" s="3">
+        <v>6</v>
+      </c>
+      <c r="D35" s="3">
+        <v>196</v>
+      </c>
+      <c r="E35" s="3">
+        <v>381</v>
+      </c>
+      <c r="F35" s="3">
+        <v>357</v>
+      </c>
+      <c r="G35" s="3">
+        <v>384</v>
+      </c>
+      <c r="H35" s="3">
+        <v>2664</v>
+      </c>
+      <c r="I35" s="3">
+        <v>384</v>
+      </c>
+      <c r="J35" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K35" s="3">
+        <v>119</v>
+      </c>
+      <c r="L35" s="3">
+        <v>304</v>
+      </c>
+      <c r="M35" s="3">
+        <v>30</v>
+      </c>
+      <c r="N35" s="3">
+        <v>2993</v>
+      </c>
+      <c r="O35" s="3">
+        <v>3903</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>45694.224363425928</v>
+      </c>
+      <c r="B36" s="3">
+        <v>8</v>
+      </c>
+      <c r="C36" s="3">
+        <v>6</v>
+      </c>
+      <c r="D36" s="3">
+        <v>196</v>
+      </c>
+      <c r="E36" s="3">
+        <v>381</v>
+      </c>
+      <c r="F36" s="3">
+        <v>357</v>
+      </c>
+      <c r="G36" s="3">
+        <v>384</v>
+      </c>
+      <c r="H36" s="3">
+        <v>2664</v>
+      </c>
+      <c r="I36" s="3">
+        <v>384</v>
+      </c>
+      <c r="J36" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K36" s="3">
+        <v>119</v>
+      </c>
+      <c r="L36" s="3">
+        <v>304</v>
+      </c>
+      <c r="M36" s="3">
+        <v>30</v>
+      </c>
+      <c r="N36" s="3">
+        <v>2993</v>
+      </c>
+      <c r="O36" s="3">
+        <v>3903</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>45694.928773148145</v>
+      </c>
+      <c r="B37" s="3">
+        <v>8</v>
+      </c>
+      <c r="C37" s="3">
+        <v>6</v>
+      </c>
+      <c r="D37" s="3">
+        <v>198</v>
+      </c>
+      <c r="E37" s="3">
+        <v>381</v>
+      </c>
+      <c r="F37" s="3">
+        <v>357</v>
+      </c>
+      <c r="G37" s="3">
+        <v>384</v>
+      </c>
+      <c r="H37" s="3">
+        <v>2664</v>
+      </c>
+      <c r="I37" s="3">
+        <v>384</v>
+      </c>
+      <c r="J37" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K37" s="3">
+        <v>119</v>
+      </c>
+      <c r="L37" s="3">
+        <v>304</v>
+      </c>
+      <c r="M37" s="3">
+        <v>30</v>
+      </c>
+      <c r="N37" s="3">
+        <v>2999</v>
+      </c>
+      <c r="O37" s="3">
+        <v>3934</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2025-02-12 @ 17:29 - v5.P.3.xlsb - 28 264 lignes - Compile OK
* modAppli.bas
- Éliminer le dernier champ de BD_Fournisseurs (fFourFMTimeStamp)* modAppli_Utils.bas
- Changer la méthode de comparer une valeur afin de s'assurer qu'il n'y a pas de fraction excédentaire aux 2 décimales
- Détruire le code associé au Conditional Formating dans 'ApplyWorksheetFormat'
- Ajout de la logique pour formater 'wshCC_Régularisations'
- Intégrer les Enum de colonnes dans toute la procédure 'ApplyWorksheetFormat'
- Ajuster la hauteur des lignes à 15 points
* modDev_Tools.bas
- Changement de nom de variable (arrOut ---> outputArr)
- Ajouter la lettre de la colonne dans le document de nomenclature des tables
* modFAC_Finale.bas
- Ajout du TimeStamp dans la table 'wshFAC_Détails' pour les types de lignes sommaire des TEC
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_File_Usage.xlsx
+++ b/DataFiles/GCF_File_Usage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8826A4B-620D-4A11-9B97-523632B8E310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AF158D-56F7-427E-A5AC-6533DD7B43BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C6563B4-B351-4CD7-B6BC-9B6B7E0B5346}"/>
   </bookViews>
@@ -484,7 +484,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B3F5A5B-0475-4A13-A512-AE71167667D2}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:O44"/>
+  <dimension ref="A1:O46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
@@ -2565,6 +2565,100 @@
         <v>4051</v>
       </c>
     </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="5">
+        <v>45700.60665509259</v>
+      </c>
+      <c r="B45" s="3">
+        <v>8</v>
+      </c>
+      <c r="C45" s="3">
+        <v>6</v>
+      </c>
+      <c r="D45" s="3">
+        <v>211</v>
+      </c>
+      <c r="E45" s="3">
+        <v>386</v>
+      </c>
+      <c r="F45" s="3">
+        <v>362</v>
+      </c>
+      <c r="G45" s="3">
+        <v>388</v>
+      </c>
+      <c r="H45" s="3">
+        <v>2681</v>
+      </c>
+      <c r="I45" s="3">
+        <v>388</v>
+      </c>
+      <c r="J45" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K45" s="3">
+        <v>119</v>
+      </c>
+      <c r="L45" s="3">
+        <v>304</v>
+      </c>
+      <c r="M45" s="3">
+        <v>30</v>
+      </c>
+      <c r="N45" s="3">
+        <v>3087</v>
+      </c>
+      <c r="O45" s="3">
+        <v>4051</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="5">
+        <v>45700.615081018521</v>
+      </c>
+      <c r="B46" s="3">
+        <v>8</v>
+      </c>
+      <c r="C46" s="3">
+        <v>6</v>
+      </c>
+      <c r="D46" s="3">
+        <v>211</v>
+      </c>
+      <c r="E46" s="3">
+        <v>386</v>
+      </c>
+      <c r="F46" s="3">
+        <v>362</v>
+      </c>
+      <c r="G46" s="3">
+        <v>388</v>
+      </c>
+      <c r="H46" s="3">
+        <v>2681</v>
+      </c>
+      <c r="I46" s="3">
+        <v>388</v>
+      </c>
+      <c r="J46" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K46" s="3">
+        <v>119</v>
+      </c>
+      <c r="L46" s="3">
+        <v>304</v>
+      </c>
+      <c r="M46" s="3">
+        <v>30</v>
+      </c>
+      <c r="N46" s="3">
+        <v>3087</v>
+      </c>
+      <c r="O46" s="3">
+        <v>4051</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2025-02-14 @ 14:10 - v5.P.5.xlsb - 28 218 lignes - Compile OK
* modAppli_Utils.bas
- Ajouter la vérification du nom de client des TEC vs. le nom du client du F/M, pour s'assurer que le clientID & le nom du client sont alignés
- Remplacer quelques numéros de colonnes par la valeur Enum correspondante
- Nouvelle sous-routine 'Vérifier_Mix_ClientID_ClientNom_TEC' pour vérifier TEC_Local (noms de clients)
* modFunctions.bas
- Changer le nom de la fonction (Fn_Get_GL_Trans_Total ---> Fn_Get_GL_Month_Trans_Total)
- Ajuster la même procédure pour retourner le total des transactions d'un mois
* modGL_Rapport.bas
- Ajouter un format pour les dates
- Ajouter un format pour le montant de la transaction
* modGL_Stats_CA.bas
 - Travail sur les statistiques du Chiffre d'Affaires
* wshFAC_Interrogation.doccls
- Ajouter un format$ pour les dates obtenues avec liste déroulante
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_File_Usage.xlsx
+++ b/DataFiles/GCF_File_Usage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED79B140-BFC5-476F-80F1-AA24857D4443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E7165D7-98B7-40F5-B5B8-DF7920F33864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C6563B4-B351-4CD7-B6BC-9B6B7E0B5346}"/>
   </bookViews>
@@ -484,7 +484,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B3F5A5B-0475-4A13-A512-AE71167667D2}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:O52"/>
+  <dimension ref="A1:O58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
@@ -2941,6 +2941,288 @@
         <v>4077</v>
       </c>
     </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A53" s="5">
+        <v>45701.931446759256</v>
+      </c>
+      <c r="B53" s="3">
+        <v>8</v>
+      </c>
+      <c r="C53" s="3">
+        <v>6</v>
+      </c>
+      <c r="D53" s="3">
+        <v>216</v>
+      </c>
+      <c r="E53" s="3">
+        <v>389</v>
+      </c>
+      <c r="F53" s="3">
+        <v>365</v>
+      </c>
+      <c r="G53" s="3">
+        <v>388</v>
+      </c>
+      <c r="H53" s="3">
+        <v>2681</v>
+      </c>
+      <c r="I53" s="3">
+        <v>388</v>
+      </c>
+      <c r="J53" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K53" s="3">
+        <v>119</v>
+      </c>
+      <c r="L53" s="3">
+        <v>304</v>
+      </c>
+      <c r="M53" s="3">
+        <v>30</v>
+      </c>
+      <c r="N53" s="3">
+        <v>3111</v>
+      </c>
+      <c r="O53" s="3">
+        <v>4116</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A54" s="5">
+        <v>45701.932812500003</v>
+      </c>
+      <c r="B54" s="3">
+        <v>8</v>
+      </c>
+      <c r="C54" s="3">
+        <v>6</v>
+      </c>
+      <c r="D54" s="3">
+        <v>216</v>
+      </c>
+      <c r="E54" s="3">
+        <v>389</v>
+      </c>
+      <c r="F54" s="3">
+        <v>365</v>
+      </c>
+      <c r="G54" s="3">
+        <v>388</v>
+      </c>
+      <c r="H54" s="3">
+        <v>2681</v>
+      </c>
+      <c r="I54" s="3">
+        <v>388</v>
+      </c>
+      <c r="J54" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K54" s="3">
+        <v>119</v>
+      </c>
+      <c r="L54" s="3">
+        <v>304</v>
+      </c>
+      <c r="M54" s="3">
+        <v>30</v>
+      </c>
+      <c r="N54" s="3">
+        <v>3111</v>
+      </c>
+      <c r="O54" s="3">
+        <v>4116</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55" s="5">
+        <v>45702.475960648146</v>
+      </c>
+      <c r="B55" s="3">
+        <v>8</v>
+      </c>
+      <c r="C55" s="3">
+        <v>6</v>
+      </c>
+      <c r="D55" s="3">
+        <v>216</v>
+      </c>
+      <c r="E55" s="3">
+        <v>389</v>
+      </c>
+      <c r="F55" s="3">
+        <v>365</v>
+      </c>
+      <c r="G55" s="3">
+        <v>388</v>
+      </c>
+      <c r="H55" s="3">
+        <v>2681</v>
+      </c>
+      <c r="I55" s="3">
+        <v>388</v>
+      </c>
+      <c r="J55" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K55" s="3">
+        <v>119</v>
+      </c>
+      <c r="L55" s="3">
+        <v>304</v>
+      </c>
+      <c r="M55" s="3">
+        <v>30</v>
+      </c>
+      <c r="N55" s="3">
+        <v>3111</v>
+      </c>
+      <c r="O55" s="3">
+        <v>4116</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A56" s="5">
+        <v>45702.479409722226</v>
+      </c>
+      <c r="B56" s="3">
+        <v>8</v>
+      </c>
+      <c r="C56" s="3">
+        <v>6</v>
+      </c>
+      <c r="D56" s="3">
+        <v>216</v>
+      </c>
+      <c r="E56" s="3">
+        <v>389</v>
+      </c>
+      <c r="F56" s="3">
+        <v>365</v>
+      </c>
+      <c r="G56" s="3">
+        <v>388</v>
+      </c>
+      <c r="H56" s="3">
+        <v>2681</v>
+      </c>
+      <c r="I56" s="3">
+        <v>388</v>
+      </c>
+      <c r="J56" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K56" s="3">
+        <v>119</v>
+      </c>
+      <c r="L56" s="3">
+        <v>304</v>
+      </c>
+      <c r="M56" s="3">
+        <v>30</v>
+      </c>
+      <c r="N56" s="3">
+        <v>3111</v>
+      </c>
+      <c r="O56" s="3">
+        <v>4116</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57" s="5">
+        <v>45702.480138888888</v>
+      </c>
+      <c r="B57" s="3">
+        <v>8</v>
+      </c>
+      <c r="C57" s="3">
+        <v>6</v>
+      </c>
+      <c r="D57" s="3">
+        <v>216</v>
+      </c>
+      <c r="E57" s="3">
+        <v>389</v>
+      </c>
+      <c r="F57" s="3">
+        <v>365</v>
+      </c>
+      <c r="G57" s="3">
+        <v>388</v>
+      </c>
+      <c r="H57" s="3">
+        <v>2681</v>
+      </c>
+      <c r="I57" s="3">
+        <v>388</v>
+      </c>
+      <c r="J57" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K57" s="3">
+        <v>119</v>
+      </c>
+      <c r="L57" s="3">
+        <v>304</v>
+      </c>
+      <c r="M57" s="3">
+        <v>30</v>
+      </c>
+      <c r="N57" s="3">
+        <v>3111</v>
+      </c>
+      <c r="O57" s="3">
+        <v>4116</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A58" s="5">
+        <v>45702.511018518519</v>
+      </c>
+      <c r="B58" s="3">
+        <v>8</v>
+      </c>
+      <c r="C58" s="3">
+        <v>6</v>
+      </c>
+      <c r="D58" s="3">
+        <v>216</v>
+      </c>
+      <c r="E58" s="3">
+        <v>389</v>
+      </c>
+      <c r="F58" s="3">
+        <v>365</v>
+      </c>
+      <c r="G58" s="3">
+        <v>388</v>
+      </c>
+      <c r="H58" s="3">
+        <v>2681</v>
+      </c>
+      <c r="I58" s="3">
+        <v>388</v>
+      </c>
+      <c r="J58" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K58" s="3">
+        <v>119</v>
+      </c>
+      <c r="L58" s="3">
+        <v>304</v>
+      </c>
+      <c r="M58" s="3">
+        <v>30</v>
+      </c>
+      <c r="N58" s="3">
+        <v>3111</v>
+      </c>
+      <c r="O58" s="3">
+        <v>4116</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2025-02-27 @ 10:17 - Clients_v5.4.xlsm - 1 561 lignes - Compile OK
* modMain.bas
- Éliminer du code en remarques
- .txtNomClientPlusNomClientSyst�me.BackColor = vbWhite n'était pas présent
- Réintégrer la mise à jour de BD_Entrée avec ADO, vérification si le fichier a été mis à jour dans les 10 dernières secondes
* modUtils.bas
- Éliminer du code en remarques
- Ajouter un 'Exit Sub' s'il y a une message d'erreur suite à la validation de la date de la dernière mise à jour
* ufClientMF.frm
- Changer le titre du userForm pour 'version 5.4'
- Ajouter une procédure liée au clic du bouton Sauvegarde qui appelle 'MAJ_Fichier_Client'
- Appel à la procédure qui écrit sur disque 'CM_Update_External_GCF_BD_Entrée' qui devient 'CM_Update_External_GCF_Entrée_BD'
- Utilisation de 'NomClientPlusNomClientSystème' plutôt que 'NomClientPlusNomSystème'
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_File_Usage.xlsx
+++ b/DataFiles/GCF_File_Usage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1349A935-145C-4E09-8C3C-ADCF407E45F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B048208-BB9C-4B84-8AB2-4BF0BABCE0D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C6563B4-B351-4CD7-B6BC-9B6B7E0B5346}"/>
   </bookViews>
@@ -484,7 +484,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B3F5A5B-0475-4A13-A512-AE71167667D2}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:O63"/>
+  <dimension ref="A1:O77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
@@ -3458,6 +3458,664 @@
         <v>4301</v>
       </c>
     </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A64" s="5">
+        <v>45711.627835648149</v>
+      </c>
+      <c r="B64" s="3">
+        <v>8</v>
+      </c>
+      <c r="C64" s="3">
+        <v>6</v>
+      </c>
+      <c r="D64" s="3">
+        <v>217</v>
+      </c>
+      <c r="E64" s="3">
+        <v>392</v>
+      </c>
+      <c r="F64" s="3">
+        <v>368</v>
+      </c>
+      <c r="G64" s="3">
+        <v>388</v>
+      </c>
+      <c r="H64" s="3">
+        <v>2681</v>
+      </c>
+      <c r="I64" s="3">
+        <v>388</v>
+      </c>
+      <c r="J64" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K64" s="3">
+        <v>119</v>
+      </c>
+      <c r="L64" s="3">
+        <v>304</v>
+      </c>
+      <c r="M64" s="3">
+        <v>30</v>
+      </c>
+      <c r="N64" s="3">
+        <v>3129</v>
+      </c>
+      <c r="O64" s="3">
+        <v>4301</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A65" s="5">
+        <v>45712.930486111109</v>
+      </c>
+      <c r="B65" s="3">
+        <v>8</v>
+      </c>
+      <c r="C65" s="3">
+        <v>6</v>
+      </c>
+      <c r="D65" s="3">
+        <v>223</v>
+      </c>
+      <c r="E65" s="3">
+        <v>393</v>
+      </c>
+      <c r="F65" s="3">
+        <v>369</v>
+      </c>
+      <c r="G65" s="3">
+        <v>388</v>
+      </c>
+      <c r="H65" s="3">
+        <v>2681</v>
+      </c>
+      <c r="I65" s="3">
+        <v>388</v>
+      </c>
+      <c r="J65" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K65" s="3">
+        <v>119</v>
+      </c>
+      <c r="L65" s="3">
+        <v>304</v>
+      </c>
+      <c r="M65" s="3">
+        <v>30</v>
+      </c>
+      <c r="N65" s="3">
+        <v>3157</v>
+      </c>
+      <c r="O65" s="3">
+        <v>4344</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A66" s="5">
+        <v>45712.93478009259</v>
+      </c>
+      <c r="B66" s="3">
+        <v>8</v>
+      </c>
+      <c r="C66" s="3">
+        <v>6</v>
+      </c>
+      <c r="D66" s="3">
+        <v>223</v>
+      </c>
+      <c r="E66" s="3">
+        <v>393</v>
+      </c>
+      <c r="F66" s="3">
+        <v>369</v>
+      </c>
+      <c r="G66" s="3">
+        <v>388</v>
+      </c>
+      <c r="H66" s="3">
+        <v>2681</v>
+      </c>
+      <c r="I66" s="3">
+        <v>388</v>
+      </c>
+      <c r="J66" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K66" s="3">
+        <v>119</v>
+      </c>
+      <c r="L66" s="3">
+        <v>304</v>
+      </c>
+      <c r="M66" s="3">
+        <v>30</v>
+      </c>
+      <c r="N66" s="3">
+        <v>3157</v>
+      </c>
+      <c r="O66" s="3">
+        <v>4344</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A67" s="5">
+        <v>45712.935312499998</v>
+      </c>
+      <c r="B67" s="3">
+        <v>8</v>
+      </c>
+      <c r="C67" s="3">
+        <v>6</v>
+      </c>
+      <c r="D67" s="3">
+        <v>223</v>
+      </c>
+      <c r="E67" s="3">
+        <v>393</v>
+      </c>
+      <c r="F67" s="3">
+        <v>369</v>
+      </c>
+      <c r="G67" s="3">
+        <v>388</v>
+      </c>
+      <c r="H67" s="3">
+        <v>2681</v>
+      </c>
+      <c r="I67" s="3">
+        <v>388</v>
+      </c>
+      <c r="J67" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K67" s="3">
+        <v>119</v>
+      </c>
+      <c r="L67" s="3">
+        <v>304</v>
+      </c>
+      <c r="M67" s="3">
+        <v>30</v>
+      </c>
+      <c r="N67" s="3">
+        <v>3157</v>
+      </c>
+      <c r="O67" s="3">
+        <v>4344</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A68" s="5">
+        <v>45713.945706018516</v>
+      </c>
+      <c r="B68" s="3">
+        <v>8</v>
+      </c>
+      <c r="C68" s="3">
+        <v>6</v>
+      </c>
+      <c r="D68" s="3">
+        <v>223</v>
+      </c>
+      <c r="E68" s="3">
+        <v>393</v>
+      </c>
+      <c r="F68" s="3">
+        <v>369</v>
+      </c>
+      <c r="G68" s="3">
+        <v>388</v>
+      </c>
+      <c r="H68" s="3">
+        <v>2681</v>
+      </c>
+      <c r="I68" s="3">
+        <v>388</v>
+      </c>
+      <c r="J68" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K68" s="3">
+        <v>119</v>
+      </c>
+      <c r="L68" s="3">
+        <v>304</v>
+      </c>
+      <c r="M68" s="3">
+        <v>30</v>
+      </c>
+      <c r="N68" s="3">
+        <v>3157</v>
+      </c>
+      <c r="O68" s="3">
+        <v>4408</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A69" s="5">
+        <v>45713.94672453704</v>
+      </c>
+      <c r="B69" s="3">
+        <v>8</v>
+      </c>
+      <c r="C69" s="3">
+        <v>6</v>
+      </c>
+      <c r="D69" s="3">
+        <v>223</v>
+      </c>
+      <c r="E69" s="3">
+        <v>393</v>
+      </c>
+      <c r="F69" s="3">
+        <v>369</v>
+      </c>
+      <c r="G69" s="3">
+        <v>388</v>
+      </c>
+      <c r="H69" s="3">
+        <v>2681</v>
+      </c>
+      <c r="I69" s="3">
+        <v>388</v>
+      </c>
+      <c r="J69" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K69" s="3">
+        <v>119</v>
+      </c>
+      <c r="L69" s="3">
+        <v>304</v>
+      </c>
+      <c r="M69" s="3">
+        <v>30</v>
+      </c>
+      <c r="N69" s="3">
+        <v>3157</v>
+      </c>
+      <c r="O69" s="3">
+        <v>4408</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A70" s="5">
+        <v>45713.948530092595</v>
+      </c>
+      <c r="B70" s="3">
+        <v>8</v>
+      </c>
+      <c r="C70" s="3">
+        <v>6</v>
+      </c>
+      <c r="D70" s="3">
+        <v>223</v>
+      </c>
+      <c r="E70" s="3">
+        <v>393</v>
+      </c>
+      <c r="F70" s="3">
+        <v>369</v>
+      </c>
+      <c r="G70" s="3">
+        <v>388</v>
+      </c>
+      <c r="H70" s="3">
+        <v>2681</v>
+      </c>
+      <c r="I70" s="3">
+        <v>388</v>
+      </c>
+      <c r="J70" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K70" s="3">
+        <v>119</v>
+      </c>
+      <c r="L70" s="3">
+        <v>304</v>
+      </c>
+      <c r="M70" s="3">
+        <v>30</v>
+      </c>
+      <c r="N70" s="3">
+        <v>3157</v>
+      </c>
+      <c r="O70" s="3">
+        <v>4408</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A71" s="5">
+        <v>45714.709872685184</v>
+      </c>
+      <c r="B71" s="3">
+        <v>8</v>
+      </c>
+      <c r="C71" s="3">
+        <v>6</v>
+      </c>
+      <c r="D71" s="3">
+        <v>244</v>
+      </c>
+      <c r="E71" s="3">
+        <v>393</v>
+      </c>
+      <c r="F71" s="3">
+        <v>369</v>
+      </c>
+      <c r="G71" s="3">
+        <v>388</v>
+      </c>
+      <c r="H71" s="3">
+        <v>2681</v>
+      </c>
+      <c r="I71" s="3">
+        <v>388</v>
+      </c>
+      <c r="J71" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K71" s="3">
+        <v>119</v>
+      </c>
+      <c r="L71" s="3">
+        <v>304</v>
+      </c>
+      <c r="M71" s="3">
+        <v>30</v>
+      </c>
+      <c r="N71" s="3">
+        <v>3232</v>
+      </c>
+      <c r="O71" s="3">
+        <v>4408</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A72" s="5">
+        <v>45714.712337962963</v>
+      </c>
+      <c r="B72" s="3">
+        <v>8</v>
+      </c>
+      <c r="C72" s="3">
+        <v>6</v>
+      </c>
+      <c r="D72" s="3">
+        <v>244</v>
+      </c>
+      <c r="E72" s="3">
+        <v>393</v>
+      </c>
+      <c r="F72" s="3">
+        <v>369</v>
+      </c>
+      <c r="G72" s="3">
+        <v>388</v>
+      </c>
+      <c r="H72" s="3">
+        <v>2681</v>
+      </c>
+      <c r="I72" s="3">
+        <v>388</v>
+      </c>
+      <c r="J72" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K72" s="3">
+        <v>119</v>
+      </c>
+      <c r="L72" s="3">
+        <v>304</v>
+      </c>
+      <c r="M72" s="3">
+        <v>30</v>
+      </c>
+      <c r="N72" s="3">
+        <v>3232</v>
+      </c>
+      <c r="O72" s="3">
+        <v>4408</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A73" s="5">
+        <v>45714.717083333337</v>
+      </c>
+      <c r="B73" s="3">
+        <v>8</v>
+      </c>
+      <c r="C73" s="3">
+        <v>6</v>
+      </c>
+      <c r="D73" s="3">
+        <v>244</v>
+      </c>
+      <c r="E73" s="3">
+        <v>393</v>
+      </c>
+      <c r="F73" s="3">
+        <v>369</v>
+      </c>
+      <c r="G73" s="3">
+        <v>388</v>
+      </c>
+      <c r="H73" s="3">
+        <v>2681</v>
+      </c>
+      <c r="I73" s="3">
+        <v>388</v>
+      </c>
+      <c r="J73" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K73" s="3">
+        <v>119</v>
+      </c>
+      <c r="L73" s="3">
+        <v>304</v>
+      </c>
+      <c r="M73" s="3">
+        <v>30</v>
+      </c>
+      <c r="N73" s="3">
+        <v>3232</v>
+      </c>
+      <c r="O73" s="3">
+        <v>4408</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A74" s="5">
+        <v>45714.725185185183</v>
+      </c>
+      <c r="B74" s="3">
+        <v>8</v>
+      </c>
+      <c r="C74" s="3">
+        <v>6</v>
+      </c>
+      <c r="D74" s="3">
+        <v>244</v>
+      </c>
+      <c r="E74" s="3">
+        <v>393</v>
+      </c>
+      <c r="F74" s="3">
+        <v>369</v>
+      </c>
+      <c r="G74" s="3">
+        <v>388</v>
+      </c>
+      <c r="H74" s="3">
+        <v>2681</v>
+      </c>
+      <c r="I74" s="3">
+        <v>388</v>
+      </c>
+      <c r="J74" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K74" s="3">
+        <v>119</v>
+      </c>
+      <c r="L74" s="3">
+        <v>304</v>
+      </c>
+      <c r="M74" s="3">
+        <v>30</v>
+      </c>
+      <c r="N74" s="3">
+        <v>3232</v>
+      </c>
+      <c r="O74" s="3">
+        <v>4408</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A75" s="5">
+        <v>45714.731226851851</v>
+      </c>
+      <c r="B75" s="3">
+        <v>8</v>
+      </c>
+      <c r="C75" s="3">
+        <v>6</v>
+      </c>
+      <c r="D75" s="3">
+        <v>244</v>
+      </c>
+      <c r="E75" s="3">
+        <v>393</v>
+      </c>
+      <c r="F75" s="3">
+        <v>369</v>
+      </c>
+      <c r="G75" s="3">
+        <v>388</v>
+      </c>
+      <c r="H75" s="3">
+        <v>2681</v>
+      </c>
+      <c r="I75" s="3">
+        <v>388</v>
+      </c>
+      <c r="J75" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K75" s="3">
+        <v>119</v>
+      </c>
+      <c r="L75" s="3">
+        <v>304</v>
+      </c>
+      <c r="M75" s="3">
+        <v>30</v>
+      </c>
+      <c r="N75" s="3">
+        <v>3232</v>
+      </c>
+      <c r="O75" s="3">
+        <v>4408</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A76" s="5">
+        <v>45714.932314814818</v>
+      </c>
+      <c r="B76" s="3">
+        <v>8</v>
+      </c>
+      <c r="C76" s="3">
+        <v>6</v>
+      </c>
+      <c r="D76" s="3">
+        <v>229</v>
+      </c>
+      <c r="E76" s="3">
+        <v>393</v>
+      </c>
+      <c r="F76" s="3">
+        <v>369</v>
+      </c>
+      <c r="G76" s="3">
+        <v>388</v>
+      </c>
+      <c r="H76" s="3">
+        <v>2681</v>
+      </c>
+      <c r="I76" s="3">
+        <v>388</v>
+      </c>
+      <c r="J76" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K76" s="3">
+        <v>119</v>
+      </c>
+      <c r="L76" s="3">
+        <v>304</v>
+      </c>
+      <c r="M76" s="3">
+        <v>30</v>
+      </c>
+      <c r="N76" s="3">
+        <v>3181</v>
+      </c>
+      <c r="O76" s="3">
+        <v>4451</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A77" s="5">
+        <v>45714.937083333331</v>
+      </c>
+      <c r="B77" s="3">
+        <v>8</v>
+      </c>
+      <c r="C77" s="3">
+        <v>6</v>
+      </c>
+      <c r="D77" s="3">
+        <v>229</v>
+      </c>
+      <c r="E77" s="3">
+        <v>393</v>
+      </c>
+      <c r="F77" s="3">
+        <v>369</v>
+      </c>
+      <c r="G77" s="3">
+        <v>388</v>
+      </c>
+      <c r="H77" s="3">
+        <v>2681</v>
+      </c>
+      <c r="I77" s="3">
+        <v>388</v>
+      </c>
+      <c r="J77" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K77" s="3">
+        <v>119</v>
+      </c>
+      <c r="L77" s="3">
+        <v>304</v>
+      </c>
+      <c r="M77" s="3">
+        <v>30</v>
+      </c>
+      <c r="N77" s="3">
+        <v>3181</v>
+      </c>
+      <c r="O77" s="3">
+        <v>4451</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2025-02-27 @ 10:57 - APP_v6.A.3.xlsb - +29 272 lignes - Compile OK
* Global
- .value a été changé pour .Value
* clsSearchableDropdown.cls
- ...Listbox a été changé pour ...ListBox
* modAppli.bas
- Éliminer du code en remarques
- Nouvel appel 'Declare PtrSafe Function GetSystemMetrics Lib "user32" (ByVal nIndex As Long) As Long'
* modAppli_Utils.bas
- Dans la validation de date, accepter les dates futures si elles sont à moins de 10 jours de la date actuelle (checkDEB_Trans & checkGL_Trans)
- Utilisation de Currency plutôt que Double
* modDEB_Saisie.bas
_ Travail et tests sur la possibilité de RENVERSER une écriture intégralement et possibilité de corriger l'entrée avant de la sauvegarder
- Utilisation de With/End With lorsque souhaitable
* Liste n'en finit plus...
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_File_Usage.xlsx
+++ b/DataFiles/GCF_File_Usage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B048208-BB9C-4B84-8AB2-4BF0BABCE0D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C150D39-47FF-42B9-9B97-A6A9567D14EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C6563B4-B351-4CD7-B6BC-9B6B7E0B5346}"/>
   </bookViews>
@@ -484,7 +484,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B3F5A5B-0475-4A13-A512-AE71167667D2}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:O77"/>
+  <dimension ref="A1:O79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
@@ -4116,6 +4116,100 @@
         <v>4451</v>
       </c>
     </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A78" s="5">
+        <v>45715.437199074076</v>
+      </c>
+      <c r="B78" s="3">
+        <v>8</v>
+      </c>
+      <c r="C78" s="3">
+        <v>6</v>
+      </c>
+      <c r="D78" s="3">
+        <v>229</v>
+      </c>
+      <c r="E78" s="3">
+        <v>393</v>
+      </c>
+      <c r="F78" s="3">
+        <v>369</v>
+      </c>
+      <c r="G78" s="3">
+        <v>388</v>
+      </c>
+      <c r="H78" s="3">
+        <v>2681</v>
+      </c>
+      <c r="I78" s="3">
+        <v>388</v>
+      </c>
+      <c r="J78" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K78" s="3">
+        <v>119</v>
+      </c>
+      <c r="L78" s="3">
+        <v>304</v>
+      </c>
+      <c r="M78" s="3">
+        <v>30</v>
+      </c>
+      <c r="N78" s="3">
+        <v>3181</v>
+      </c>
+      <c r="O78" s="3">
+        <v>4451</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A79" s="5">
+        <v>45715.438310185185</v>
+      </c>
+      <c r="B79" s="3">
+        <v>8</v>
+      </c>
+      <c r="C79" s="3">
+        <v>6</v>
+      </c>
+      <c r="D79" s="3">
+        <v>229</v>
+      </c>
+      <c r="E79" s="3">
+        <v>393</v>
+      </c>
+      <c r="F79" s="3">
+        <v>369</v>
+      </c>
+      <c r="G79" s="3">
+        <v>388</v>
+      </c>
+      <c r="H79" s="3">
+        <v>2681</v>
+      </c>
+      <c r="I79" s="3">
+        <v>388</v>
+      </c>
+      <c r="J79" s="3">
+        <v>1216</v>
+      </c>
+      <c r="K79" s="3">
+        <v>119</v>
+      </c>
+      <c r="L79" s="3">
+        <v>304</v>
+      </c>
+      <c r="M79" s="3">
+        <v>30</v>
+      </c>
+      <c r="N79" s="3">
+        <v>3181</v>
+      </c>
+      <c r="O79" s="3">
+        <v>4451</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2025-03-01 @ 13:40 - v6.A.5.xlsb - 28 249 lignes - Compile OK
* modFAC_Interrogation.bas
- Plage ---> plage
* modFunctions.bas
- Nouvelle fonction pour déterminer s'il y a ou pas de lignes sélectionnée dans un listBox
* modGL_EJ.bas
- Changer le tri des écritures de journal (No. Entrée, Débit (D) et Crédit (D)
* modGL_PrepEF.bas
- Éliminer du code en remarques
* modGL_Rapport_Nouveau.bas
- Nouveau module pour la refonte du rapport des transactions du G/L (570 lignes)
* modGL_Rapport_TBD.bas
- Ce module devient inutile, toutes les lignes en remarques
* modMENU_GL.bas
- Appel au userForm 'ufGL_Rapport' plutôt que la feuille wshGL_Rapport
* ufGL_Rapport
- Nouveau userForm pour saisir les paramètres du rapport (228 lignes)
* wshGL_Rapport.doccls
- Feuille désuète, mise en remarques de tout le code
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_File_Usage.xlsx
+++ b/DataFiles/GCF_File_Usage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C150D39-47FF-42B9-9B97-A6A9567D14EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51293AEA-F01E-4449-A8AC-A734A704F667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C6563B4-B351-4CD7-B6BC-9B6B7E0B5346}"/>
   </bookViews>
@@ -484,7 +484,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B3F5A5B-0475-4A13-A512-AE71167667D2}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:O79"/>
+  <dimension ref="A1:O81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
@@ -4210,6 +4210,100 @@
         <v>4451</v>
       </c>
     </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A80" s="5">
+        <v>45716.900231481479</v>
+      </c>
+      <c r="B80" s="3">
+        <v>8</v>
+      </c>
+      <c r="C80" s="3">
+        <v>6</v>
+      </c>
+      <c r="D80" s="3">
+        <v>229</v>
+      </c>
+      <c r="E80" s="3">
+        <v>393</v>
+      </c>
+      <c r="F80" s="3">
+        <v>369</v>
+      </c>
+      <c r="G80" s="3">
+        <v>388</v>
+      </c>
+      <c r="H80" s="3">
+        <v>2681</v>
+      </c>
+      <c r="I80" s="3">
+        <v>388</v>
+      </c>
+      <c r="J80" s="3">
+        <v>2022</v>
+      </c>
+      <c r="K80" s="3">
+        <v>207</v>
+      </c>
+      <c r="L80" s="3">
+        <v>304</v>
+      </c>
+      <c r="M80" s="3">
+        <v>30</v>
+      </c>
+      <c r="N80" s="3">
+        <v>3189</v>
+      </c>
+      <c r="O80" s="3">
+        <v>4532</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A81" s="5">
+        <v>45716.901041666664</v>
+      </c>
+      <c r="B81" s="3">
+        <v>8</v>
+      </c>
+      <c r="C81" s="3">
+        <v>6</v>
+      </c>
+      <c r="D81" s="3">
+        <v>229</v>
+      </c>
+      <c r="E81" s="3">
+        <v>393</v>
+      </c>
+      <c r="F81" s="3">
+        <v>369</v>
+      </c>
+      <c r="G81" s="3">
+        <v>388</v>
+      </c>
+      <c r="H81" s="3">
+        <v>2681</v>
+      </c>
+      <c r="I81" s="3">
+        <v>388</v>
+      </c>
+      <c r="J81" s="3">
+        <v>2022</v>
+      </c>
+      <c r="K81" s="3">
+        <v>207</v>
+      </c>
+      <c r="L81" s="3">
+        <v>304</v>
+      </c>
+      <c r="M81" s="3">
+        <v>30</v>
+      </c>
+      <c r="N81" s="3">
+        <v>3189</v>
+      </c>
+      <c r="O81" s="3">
+        <v>4532</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2025-03-05 @ 07:57 - v5.4.xlsm - 1 629 lignes - Compile OK
Ajout des annotations @Folder("Gestion_Clients")
* modFunctions.bas
- Changer la structure de l'appel de MsgBox (Prompt, Title & Buttons)
- Utilisation de la nouvelle fonction qui normalise le champ adresse courriel
- Changer ByVal ---> ByRef pour la variable courriel dans la fonction 'Fn_ValiderCourriel'
- Nouvelle fonction 'Fn_NormaliserAdressesCourriel' pour corriger la structure du champs adresse courriel
* modMain.bas
- Utilisation de 'Application.WorksheetFunction.CountA(Sheets("Donn�es").Range("A:A"))' plutôt que '[Counta(Donn�es!A:A)]'
- Utilisation du codeName plutôt que le nom de la feuille
* modUtils.bas
- Éliminer l'assignation de la valeur 'r'
* ufClientMF.frm
- Encapsulation de Propriétés (EnableEvents, NouveauClient, IsActiveSearch
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_File_Usage.xlsx
+++ b/DataFiles/GCF_File_Usage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A02871A-3C86-4021-846B-22ABADA53B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63828D75-70D4-4FD1-ABF9-1DA82A27DA97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C6563B4-B351-4CD7-B6BC-9B6B7E0B5346}"/>
   </bookViews>
@@ -484,7 +484,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B3F5A5B-0475-4A13-A512-AE71167667D2}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:O84"/>
+  <dimension ref="A1:O85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
@@ -4445,6 +4445,53 @@
         <v>4570</v>
       </c>
     </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A85" s="5">
+        <v>45720.93949074074</v>
+      </c>
+      <c r="B85" s="3">
+        <v>10</v>
+      </c>
+      <c r="C85" s="3">
+        <v>6</v>
+      </c>
+      <c r="D85" s="3">
+        <v>235</v>
+      </c>
+      <c r="E85" s="3">
+        <v>411</v>
+      </c>
+      <c r="F85" s="3">
+        <v>387</v>
+      </c>
+      <c r="G85" s="3">
+        <v>474</v>
+      </c>
+      <c r="H85" s="3">
+        <v>3381</v>
+      </c>
+      <c r="I85" s="3">
+        <v>474</v>
+      </c>
+      <c r="J85" s="3">
+        <v>2026</v>
+      </c>
+      <c r="K85" s="3">
+        <v>208</v>
+      </c>
+      <c r="L85" s="3">
+        <v>415</v>
+      </c>
+      <c r="M85" s="3">
+        <v>30</v>
+      </c>
+      <c r="N85" s="3">
+        <v>3612</v>
+      </c>
+      <c r="O85" s="3">
+        <v>4604</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2025-03-10 @ 16:56 - v6.B.4.xlsb - 29 199 lignes - Compile OK
* Suite à l'analyse de RubberDuck, quelques insertions de remarques:
- '@IgnoreModule UnassignedVariableUsage
- '@Ignore UnassignedVariableUsage
* modDev_Tools.bas
- Procédure 'ExporterCodeVBA' - Ajustement du code pour exporter le codes feuilles
* modImport.bas
- Procédure 'FAC_Entête_Import_All' - Ajustement pour faire un resize après l'import de la table FAC_Entête de GCF_BD_MASTER
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_File_Usage.xlsx
+++ b/DataFiles/GCF_File_Usage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6577FB-BAFE-4BE2-BCAD-45C387D88C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC1A0A1-1647-44F4-AB34-2D41C6AF5ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C6563B4-B351-4CD7-B6BC-9B6B7E0B5346}"/>
   </bookViews>
@@ -484,7 +484,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B3F5A5B-0475-4A13-A512-AE71167667D2}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:O91"/>
+  <dimension ref="A1:O100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
@@ -4774,6 +4774,429 @@
         <v>4686</v>
       </c>
     </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A92" s="5">
+        <v>45725.733101851853</v>
+      </c>
+      <c r="B92" s="3">
+        <v>10</v>
+      </c>
+      <c r="C92" s="3">
+        <v>6</v>
+      </c>
+      <c r="D92" s="3">
+        <v>240</v>
+      </c>
+      <c r="E92" s="3">
+        <v>423</v>
+      </c>
+      <c r="F92" s="3">
+        <v>399</v>
+      </c>
+      <c r="G92" s="3">
+        <v>476</v>
+      </c>
+      <c r="H92" s="3">
+        <v>3432</v>
+      </c>
+      <c r="I92" s="3">
+        <v>476</v>
+      </c>
+      <c r="J92" s="3">
+        <v>2026</v>
+      </c>
+      <c r="K92" s="3">
+        <v>208</v>
+      </c>
+      <c r="L92" s="3">
+        <v>417</v>
+      </c>
+      <c r="M92" s="3">
+        <v>30</v>
+      </c>
+      <c r="N92" s="3">
+        <v>3667</v>
+      </c>
+      <c r="O92" s="3">
+        <v>4686</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A93" s="5">
+        <v>45725.737037037034</v>
+      </c>
+      <c r="B93" s="3">
+        <v>10</v>
+      </c>
+      <c r="C93" s="3">
+        <v>6</v>
+      </c>
+      <c r="D93" s="3">
+        <v>240</v>
+      </c>
+      <c r="E93" s="3">
+        <v>423</v>
+      </c>
+      <c r="F93" s="3">
+        <v>399</v>
+      </c>
+      <c r="G93" s="3">
+        <v>476</v>
+      </c>
+      <c r="H93" s="3">
+        <v>3432</v>
+      </c>
+      <c r="I93" s="3">
+        <v>476</v>
+      </c>
+      <c r="J93" s="3">
+        <v>2026</v>
+      </c>
+      <c r="K93" s="3">
+        <v>208</v>
+      </c>
+      <c r="L93" s="3">
+        <v>417</v>
+      </c>
+      <c r="M93" s="3">
+        <v>30</v>
+      </c>
+      <c r="N93" s="3">
+        <v>3667</v>
+      </c>
+      <c r="O93" s="3">
+        <v>4686</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A94" s="5">
+        <v>45725.739548611113</v>
+      </c>
+      <c r="B94" s="3">
+        <v>10</v>
+      </c>
+      <c r="C94" s="3">
+        <v>6</v>
+      </c>
+      <c r="D94" s="3">
+        <v>240</v>
+      </c>
+      <c r="E94" s="3">
+        <v>423</v>
+      </c>
+      <c r="F94" s="3">
+        <v>399</v>
+      </c>
+      <c r="G94" s="3">
+        <v>476</v>
+      </c>
+      <c r="H94" s="3">
+        <v>3432</v>
+      </c>
+      <c r="I94" s="3">
+        <v>476</v>
+      </c>
+      <c r="J94" s="3">
+        <v>2026</v>
+      </c>
+      <c r="K94" s="3">
+        <v>208</v>
+      </c>
+      <c r="L94" s="3">
+        <v>417</v>
+      </c>
+      <c r="M94" s="3">
+        <v>30</v>
+      </c>
+      <c r="N94" s="3">
+        <v>3667</v>
+      </c>
+      <c r="O94" s="3">
+        <v>4686</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A95" s="5">
+        <v>45725.742303240739</v>
+      </c>
+      <c r="B95" s="3">
+        <v>10</v>
+      </c>
+      <c r="C95" s="3">
+        <v>6</v>
+      </c>
+      <c r="D95" s="3">
+        <v>240</v>
+      </c>
+      <c r="E95" s="3">
+        <v>423</v>
+      </c>
+      <c r="F95" s="3">
+        <v>399</v>
+      </c>
+      <c r="G95" s="3">
+        <v>476</v>
+      </c>
+      <c r="H95" s="3">
+        <v>3432</v>
+      </c>
+      <c r="I95" s="3">
+        <v>476</v>
+      </c>
+      <c r="J95" s="3">
+        <v>2026</v>
+      </c>
+      <c r="K95" s="3">
+        <v>208</v>
+      </c>
+      <c r="L95" s="3">
+        <v>417</v>
+      </c>
+      <c r="M95" s="3">
+        <v>30</v>
+      </c>
+      <c r="N95" s="3">
+        <v>3667</v>
+      </c>
+      <c r="O95" s="3">
+        <v>4686</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A96" s="5">
+        <v>45725.743796296294</v>
+      </c>
+      <c r="B96" s="3">
+        <v>10</v>
+      </c>
+      <c r="C96" s="3">
+        <v>6</v>
+      </c>
+      <c r="D96" s="3">
+        <v>240</v>
+      </c>
+      <c r="E96" s="3">
+        <v>423</v>
+      </c>
+      <c r="F96" s="3">
+        <v>399</v>
+      </c>
+      <c r="G96" s="3">
+        <v>476</v>
+      </c>
+      <c r="H96" s="3">
+        <v>3432</v>
+      </c>
+      <c r="I96" s="3">
+        <v>476</v>
+      </c>
+      <c r="J96" s="3">
+        <v>2026</v>
+      </c>
+      <c r="K96" s="3">
+        <v>208</v>
+      </c>
+      <c r="L96" s="3">
+        <v>417</v>
+      </c>
+      <c r="M96" s="3">
+        <v>30</v>
+      </c>
+      <c r="N96" s="3">
+        <v>3667</v>
+      </c>
+      <c r="O96" s="3">
+        <v>4686</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A97" s="5">
+        <v>45725.769189814811</v>
+      </c>
+      <c r="B97" s="3">
+        <v>10</v>
+      </c>
+      <c r="C97" s="3">
+        <v>6</v>
+      </c>
+      <c r="D97" s="3">
+        <v>240</v>
+      </c>
+      <c r="E97" s="3">
+        <v>423</v>
+      </c>
+      <c r="F97" s="3">
+        <v>399</v>
+      </c>
+      <c r="G97" s="3">
+        <v>476</v>
+      </c>
+      <c r="H97" s="3">
+        <v>3432</v>
+      </c>
+      <c r="I97" s="3">
+        <v>476</v>
+      </c>
+      <c r="J97" s="3">
+        <v>2026</v>
+      </c>
+      <c r="K97" s="3">
+        <v>208</v>
+      </c>
+      <c r="L97" s="3">
+        <v>417</v>
+      </c>
+      <c r="M97" s="3">
+        <v>30</v>
+      </c>
+      <c r="N97" s="3">
+        <v>3667</v>
+      </c>
+      <c r="O97" s="3">
+        <v>4686</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A98" s="5">
+        <v>45725.784131944441</v>
+      </c>
+      <c r="B98" s="3">
+        <v>10</v>
+      </c>
+      <c r="C98" s="3">
+        <v>6</v>
+      </c>
+      <c r="D98" s="3">
+        <v>240</v>
+      </c>
+      <c r="E98" s="3">
+        <v>423</v>
+      </c>
+      <c r="F98" s="3">
+        <v>399</v>
+      </c>
+      <c r="G98" s="3">
+        <v>476</v>
+      </c>
+      <c r="H98" s="3">
+        <v>3432</v>
+      </c>
+      <c r="I98" s="3">
+        <v>476</v>
+      </c>
+      <c r="J98" s="3">
+        <v>2026</v>
+      </c>
+      <c r="K98" s="3">
+        <v>208</v>
+      </c>
+      <c r="L98" s="3">
+        <v>417</v>
+      </c>
+      <c r="M98" s="3">
+        <v>30</v>
+      </c>
+      <c r="N98" s="3">
+        <v>3667</v>
+      </c>
+      <c r="O98" s="3">
+        <v>4686</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A99" s="5">
+        <v>45725.784699074073</v>
+      </c>
+      <c r="B99" s="3">
+        <v>10</v>
+      </c>
+      <c r="C99" s="3">
+        <v>6</v>
+      </c>
+      <c r="D99" s="3">
+        <v>240</v>
+      </c>
+      <c r="E99" s="3">
+        <v>423</v>
+      </c>
+      <c r="F99" s="3">
+        <v>399</v>
+      </c>
+      <c r="G99" s="3">
+        <v>476</v>
+      </c>
+      <c r="H99" s="3">
+        <v>3432</v>
+      </c>
+      <c r="I99" s="3">
+        <v>476</v>
+      </c>
+      <c r="J99" s="3">
+        <v>2026</v>
+      </c>
+      <c r="K99" s="3">
+        <v>208</v>
+      </c>
+      <c r="L99" s="3">
+        <v>417</v>
+      </c>
+      <c r="M99" s="3">
+        <v>30</v>
+      </c>
+      <c r="N99" s="3">
+        <v>3667</v>
+      </c>
+      <c r="O99" s="3">
+        <v>4686</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A100" s="5">
+        <v>45725.786273148151</v>
+      </c>
+      <c r="B100" s="3">
+        <v>10</v>
+      </c>
+      <c r="C100" s="3">
+        <v>6</v>
+      </c>
+      <c r="D100" s="3">
+        <v>240</v>
+      </c>
+      <c r="E100" s="3">
+        <v>423</v>
+      </c>
+      <c r="F100" s="3">
+        <v>399</v>
+      </c>
+      <c r="G100" s="3">
+        <v>476</v>
+      </c>
+      <c r="H100" s="3">
+        <v>3432</v>
+      </c>
+      <c r="I100" s="3">
+        <v>476</v>
+      </c>
+      <c r="J100" s="3">
+        <v>2026</v>
+      </c>
+      <c r="K100" s="3">
+        <v>208</v>
+      </c>
+      <c r="L100" s="3">
+        <v>417</v>
+      </c>
+      <c r="M100" s="3">
+        <v>30</v>
+      </c>
+      <c r="N100" s="3">
+        <v>3667</v>
+      </c>
+      <c r="O100" s="3">
+        <v>4686</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2025-03-11 @ 08:12 - v6.B.5.xlsb - 29 276 lignes - Compile OK
* Refactoring
- Toutes les procédures d'import (MASTER @ Local) ont été renommées, et les appels se font maintenant dans la forme 'module.procédure'
* modAppli.bas
- Recommendation de RubberDuck, de changer le type de variable de Integer @ Long
- Éliminer des variables déclarées, mais non utilisées
- Dans la procédure 'checkTEC' éliminer la vérification du client TEC vs. Client fichier-maître (Il est possible que le nom change dans le fichier maître)
* modImport.bas
- Toutes les procédures ont été renommées 'Importer...'
- 'ResizeTable' ---> 'RedimensionnerTable'
- 'ApplyFormatting' ---> 'AppliquerStyleTable'
- Modification de l'import de certaines tables pour s'assurer que des lignes vides ne soient pas laissées dans la table qui reçoit les données
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_File_Usage.xlsx
+++ b/DataFiles/GCF_File_Usage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC1A0A1-1647-44F4-AB34-2D41C6AF5ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864AB360-D0F4-4F10-95E9-96EE7EB37EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C6563B4-B351-4CD7-B6BC-9B6B7E0B5346}"/>
   </bookViews>
@@ -484,7 +484,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B3F5A5B-0475-4A13-A512-AE71167667D2}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:O100"/>
+  <dimension ref="A1:O109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
@@ -5197,6 +5197,429 @@
         <v>4686</v>
       </c>
     </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A101" s="5">
+        <v>45726.720196759263</v>
+      </c>
+      <c r="B101" s="3">
+        <v>10</v>
+      </c>
+      <c r="C101" s="3">
+        <v>6</v>
+      </c>
+      <c r="D101" s="3">
+        <v>240</v>
+      </c>
+      <c r="E101" s="3">
+        <v>426</v>
+      </c>
+      <c r="F101" s="3">
+        <v>402</v>
+      </c>
+      <c r="G101" s="3">
+        <v>476</v>
+      </c>
+      <c r="H101" s="3">
+        <v>3432</v>
+      </c>
+      <c r="I101" s="3">
+        <v>476</v>
+      </c>
+      <c r="J101" s="3">
+        <v>2026</v>
+      </c>
+      <c r="K101" s="3">
+        <v>208</v>
+      </c>
+      <c r="L101" s="3">
+        <v>417</v>
+      </c>
+      <c r="M101" s="3">
+        <v>30</v>
+      </c>
+      <c r="N101" s="3">
+        <v>3683</v>
+      </c>
+      <c r="O101" s="3">
+        <v>4702</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A102" s="5">
+        <v>45726.721956018519</v>
+      </c>
+      <c r="B102" s="3">
+        <v>10</v>
+      </c>
+      <c r="C102" s="3">
+        <v>6</v>
+      </c>
+      <c r="D102" s="3">
+        <v>240</v>
+      </c>
+      <c r="E102" s="3">
+        <v>426</v>
+      </c>
+      <c r="F102" s="3">
+        <v>402</v>
+      </c>
+      <c r="G102" s="3">
+        <v>476</v>
+      </c>
+      <c r="H102" s="3">
+        <v>3432</v>
+      </c>
+      <c r="I102" s="3">
+        <v>476</v>
+      </c>
+      <c r="J102" s="3">
+        <v>2026</v>
+      </c>
+      <c r="K102" s="3">
+        <v>208</v>
+      </c>
+      <c r="L102" s="3">
+        <v>417</v>
+      </c>
+      <c r="M102" s="3">
+        <v>30</v>
+      </c>
+      <c r="N102" s="3">
+        <v>3683</v>
+      </c>
+      <c r="O102" s="3">
+        <v>4702</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A103" s="5">
+        <v>45727.226168981484</v>
+      </c>
+      <c r="B103" s="3">
+        <v>10</v>
+      </c>
+      <c r="C103" s="3">
+        <v>6</v>
+      </c>
+      <c r="D103" s="3">
+        <v>240</v>
+      </c>
+      <c r="E103" s="3">
+        <v>426</v>
+      </c>
+      <c r="F103" s="3">
+        <v>402</v>
+      </c>
+      <c r="G103" s="3">
+        <v>476</v>
+      </c>
+      <c r="H103" s="3">
+        <v>3432</v>
+      </c>
+      <c r="I103" s="3">
+        <v>476</v>
+      </c>
+      <c r="J103" s="3">
+        <v>2026</v>
+      </c>
+      <c r="K103" s="3">
+        <v>208</v>
+      </c>
+      <c r="L103" s="3">
+        <v>417</v>
+      </c>
+      <c r="M103" s="3">
+        <v>30</v>
+      </c>
+      <c r="N103" s="3">
+        <v>3683</v>
+      </c>
+      <c r="O103" s="3">
+        <v>4725</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A104" s="5">
+        <v>45727.233865740738</v>
+      </c>
+      <c r="B104" s="3">
+        <v>10</v>
+      </c>
+      <c r="C104" s="3">
+        <v>6</v>
+      </c>
+      <c r="D104" s="3">
+        <v>240</v>
+      </c>
+      <c r="E104" s="3">
+        <v>426</v>
+      </c>
+      <c r="F104" s="3">
+        <v>402</v>
+      </c>
+      <c r="G104" s="3">
+        <v>476</v>
+      </c>
+      <c r="H104" s="3">
+        <v>3432</v>
+      </c>
+      <c r="I104" s="3">
+        <v>476</v>
+      </c>
+      <c r="J104" s="3">
+        <v>2026</v>
+      </c>
+      <c r="K104" s="3">
+        <v>208</v>
+      </c>
+      <c r="L104" s="3">
+        <v>417</v>
+      </c>
+      <c r="M104" s="3">
+        <v>30</v>
+      </c>
+      <c r="N104" s="3">
+        <v>3683</v>
+      </c>
+      <c r="O104" s="3">
+        <v>4725</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A105" s="5">
+        <v>45727.237384259257</v>
+      </c>
+      <c r="B105" s="3">
+        <v>10</v>
+      </c>
+      <c r="C105" s="3">
+        <v>6</v>
+      </c>
+      <c r="D105" s="3">
+        <v>240</v>
+      </c>
+      <c r="E105" s="3">
+        <v>426</v>
+      </c>
+      <c r="F105" s="3">
+        <v>402</v>
+      </c>
+      <c r="G105" s="3">
+        <v>476</v>
+      </c>
+      <c r="H105" s="3">
+        <v>3432</v>
+      </c>
+      <c r="I105" s="3">
+        <v>476</v>
+      </c>
+      <c r="J105" s="3">
+        <v>2026</v>
+      </c>
+      <c r="K105" s="3">
+        <v>208</v>
+      </c>
+      <c r="L105" s="3">
+        <v>417</v>
+      </c>
+      <c r="M105" s="3">
+        <v>30</v>
+      </c>
+      <c r="N105" s="3">
+        <v>3683</v>
+      </c>
+      <c r="O105" s="3">
+        <v>4725</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A106" s="5">
+        <v>45727.24659722222</v>
+      </c>
+      <c r="B106" s="3">
+        <v>10</v>
+      </c>
+      <c r="C106" s="3">
+        <v>6</v>
+      </c>
+      <c r="D106" s="3">
+        <v>240</v>
+      </c>
+      <c r="E106" s="3">
+        <v>426</v>
+      </c>
+      <c r="F106" s="3">
+        <v>402</v>
+      </c>
+      <c r="G106" s="3">
+        <v>476</v>
+      </c>
+      <c r="H106" s="3">
+        <v>3432</v>
+      </c>
+      <c r="I106" s="3">
+        <v>476</v>
+      </c>
+      <c r="J106" s="3">
+        <v>2026</v>
+      </c>
+      <c r="K106" s="3">
+        <v>208</v>
+      </c>
+      <c r="L106" s="3">
+        <v>417</v>
+      </c>
+      <c r="M106" s="3">
+        <v>30</v>
+      </c>
+      <c r="N106" s="3">
+        <v>3683</v>
+      </c>
+      <c r="O106" s="3">
+        <v>4725</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A107" s="5">
+        <v>45727.298449074071</v>
+      </c>
+      <c r="B107" s="3">
+        <v>10</v>
+      </c>
+      <c r="C107" s="3">
+        <v>6</v>
+      </c>
+      <c r="D107" s="3">
+        <v>240</v>
+      </c>
+      <c r="E107" s="3">
+        <v>426</v>
+      </c>
+      <c r="F107" s="3">
+        <v>402</v>
+      </c>
+      <c r="G107" s="3">
+        <v>476</v>
+      </c>
+      <c r="H107" s="3">
+        <v>3432</v>
+      </c>
+      <c r="I107" s="3">
+        <v>476</v>
+      </c>
+      <c r="J107" s="3">
+        <v>2026</v>
+      </c>
+      <c r="K107" s="3">
+        <v>208</v>
+      </c>
+      <c r="L107" s="3">
+        <v>417</v>
+      </c>
+      <c r="M107" s="3">
+        <v>30</v>
+      </c>
+      <c r="N107" s="3">
+        <v>3683</v>
+      </c>
+      <c r="O107" s="3">
+        <v>4725</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A108" s="5">
+        <v>45727.304571759261</v>
+      </c>
+      <c r="B108" s="3">
+        <v>10</v>
+      </c>
+      <c r="C108" s="3">
+        <v>6</v>
+      </c>
+      <c r="D108" s="3">
+        <v>240</v>
+      </c>
+      <c r="E108" s="3">
+        <v>426</v>
+      </c>
+      <c r="F108" s="3">
+        <v>402</v>
+      </c>
+      <c r="G108" s="3">
+        <v>476</v>
+      </c>
+      <c r="H108" s="3">
+        <v>3432</v>
+      </c>
+      <c r="I108" s="3">
+        <v>476</v>
+      </c>
+      <c r="J108" s="3">
+        <v>2026</v>
+      </c>
+      <c r="K108" s="3">
+        <v>208</v>
+      </c>
+      <c r="L108" s="3">
+        <v>417</v>
+      </c>
+      <c r="M108" s="3">
+        <v>30</v>
+      </c>
+      <c r="N108" s="3">
+        <v>3683</v>
+      </c>
+      <c r="O108" s="3">
+        <v>4725</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A109" s="5">
+        <v>45727.33902777778</v>
+      </c>
+      <c r="B109" s="3">
+        <v>10</v>
+      </c>
+      <c r="C109" s="3">
+        <v>6</v>
+      </c>
+      <c r="D109" s="3">
+        <v>240</v>
+      </c>
+      <c r="E109" s="3">
+        <v>426</v>
+      </c>
+      <c r="F109" s="3">
+        <v>402</v>
+      </c>
+      <c r="G109" s="3">
+        <v>476</v>
+      </c>
+      <c r="H109" s="3">
+        <v>3432</v>
+      </c>
+      <c r="I109" s="3">
+        <v>476</v>
+      </c>
+      <c r="J109" s="3">
+        <v>2026</v>
+      </c>
+      <c r="K109" s="3">
+        <v>208</v>
+      </c>
+      <c r="L109" s="3">
+        <v>417</v>
+      </c>
+      <c r="M109" s="3">
+        <v>30</v>
+      </c>
+      <c r="N109" s="3">
+        <v>3683</v>
+      </c>
+      <c r="O109" s="3">
+        <v>4725</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2025-03-12 @ 13:02 - v6.C.xlsb - 29 441 lignes - Compile OK
* Architecture
- Changement des feuilles de données de 'wsh' ---> 'wsd'
- Ajout d'un séparateur (toutes les feuilles de données sont à gauche de celui-ci)
- Déplacer toutes les feuilles de type Doc vers la droite
- Déplacer toutes les feuilles de type Menu vers la droite
- 'UserForm_Params' devient 'Doc_UserForm_Params'
* Variable globale
- gPreviousCellAddress (enlever la déclaration dans plusieurs modules)
* modFAC_Confirmation.bas
- Ménage dans le code (maintenant on utilise un userForm plutôt qu'une feuille (beaucoup de code 'CommentOut')
* ThisWorkbook.doccls
- Ajout d'une remarque
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_File_Usage.xlsx
+++ b/DataFiles/GCF_File_Usage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C1FBA1-4C1C-44C4-A0AE-DA1007921B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6882C135-5A61-47E5-A8B6-FA7C7A68008C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C6563B4-B351-4CD7-B6BC-9B6B7E0B5346}"/>
   </bookViews>
@@ -484,7 +484,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B3F5A5B-0475-4A13-A512-AE71167667D2}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
@@ -1343,6 +1343,53 @@
         <v>4725</v>
       </c>
     </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>45728.502708333333</v>
+      </c>
+      <c r="B19" s="3">
+        <v>10</v>
+      </c>
+      <c r="C19" s="3">
+        <v>6</v>
+      </c>
+      <c r="D19" s="3">
+        <v>240</v>
+      </c>
+      <c r="E19" s="3">
+        <v>426</v>
+      </c>
+      <c r="F19" s="3">
+        <v>402</v>
+      </c>
+      <c r="G19" s="3">
+        <v>476</v>
+      </c>
+      <c r="H19" s="3">
+        <v>3432</v>
+      </c>
+      <c r="I19" s="3">
+        <v>476</v>
+      </c>
+      <c r="J19" s="3">
+        <v>2026</v>
+      </c>
+      <c r="K19" s="3">
+        <v>208</v>
+      </c>
+      <c r="L19" s="3">
+        <v>417</v>
+      </c>
+      <c r="M19" s="3">
+        <v>30</v>
+      </c>
+      <c r="N19" s="3">
+        <v>3683</v>
+      </c>
+      <c r="O19" s="3">
+        <v>4725</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2025-03-18 @ 10:42 - Avant compare
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_File_Usage.xlsx
+++ b/DataFiles/GCF_File_Usage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE5BC42-6000-4F17-BF97-DA8C8010E874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29286260-B123-4ED5-AA3F-63DA633282C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C6563B4-B351-4CD7-B6BC-9B6B7E0B5346}"/>
   </bookViews>
@@ -484,7 +484,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B3F5A5B-0475-4A13-A512-AE71167667D2}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
@@ -1625,6 +1625,147 @@
         <v>4832</v>
       </c>
     </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>45732.698807870373</v>
+      </c>
+      <c r="B25" s="3">
+        <v>10</v>
+      </c>
+      <c r="C25" s="3">
+        <v>6</v>
+      </c>
+      <c r="D25" s="3">
+        <v>249</v>
+      </c>
+      <c r="E25" s="3">
+        <v>440</v>
+      </c>
+      <c r="F25" s="3">
+        <v>416</v>
+      </c>
+      <c r="G25" s="3">
+        <v>476</v>
+      </c>
+      <c r="H25" s="3">
+        <v>3432</v>
+      </c>
+      <c r="I25" s="3">
+        <v>476</v>
+      </c>
+      <c r="J25" s="3">
+        <v>2026</v>
+      </c>
+      <c r="K25" s="3">
+        <v>208</v>
+      </c>
+      <c r="L25" s="3">
+        <v>417</v>
+      </c>
+      <c r="M25" s="3">
+        <v>30</v>
+      </c>
+      <c r="N25" s="3">
+        <v>3765</v>
+      </c>
+      <c r="O25" s="3">
+        <v>4892</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>45732.700601851851</v>
+      </c>
+      <c r="B26" s="3">
+        <v>10</v>
+      </c>
+      <c r="C26" s="3">
+        <v>6</v>
+      </c>
+      <c r="D26" s="3">
+        <v>249</v>
+      </c>
+      <c r="E26" s="3">
+        <v>440</v>
+      </c>
+      <c r="F26" s="3">
+        <v>416</v>
+      </c>
+      <c r="G26" s="3">
+        <v>476</v>
+      </c>
+      <c r="H26" s="3">
+        <v>3432</v>
+      </c>
+      <c r="I26" s="3">
+        <v>476</v>
+      </c>
+      <c r="J26" s="3">
+        <v>2026</v>
+      </c>
+      <c r="K26" s="3">
+        <v>208</v>
+      </c>
+      <c r="L26" s="3">
+        <v>417</v>
+      </c>
+      <c r="M26" s="3">
+        <v>30</v>
+      </c>
+      <c r="N26" s="3">
+        <v>3765</v>
+      </c>
+      <c r="O26" s="3">
+        <v>4892</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>45732.702893518515</v>
+      </c>
+      <c r="B27" s="3">
+        <v>10</v>
+      </c>
+      <c r="C27" s="3">
+        <v>6</v>
+      </c>
+      <c r="D27" s="3">
+        <v>249</v>
+      </c>
+      <c r="E27" s="3">
+        <v>440</v>
+      </c>
+      <c r="F27" s="3">
+        <v>416</v>
+      </c>
+      <c r="G27" s="3">
+        <v>476</v>
+      </c>
+      <c r="H27" s="3">
+        <v>3432</v>
+      </c>
+      <c r="I27" s="3">
+        <v>476</v>
+      </c>
+      <c r="J27" s="3">
+        <v>2026</v>
+      </c>
+      <c r="K27" s="3">
+        <v>208</v>
+      </c>
+      <c r="L27" s="3">
+        <v>417</v>
+      </c>
+      <c r="M27" s="3">
+        <v>30</v>
+      </c>
+      <c r="N27" s="3">
+        <v>3765</v>
+      </c>
+      <c r="O27" s="3">
+        <v>4892</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2025-03-19 @ 04:37 - v6.C.2.xlsb - 29 55 lignes - Compile OK
* Casse
- .ListBox ---> .listBox
* modAppli_Utils.bas
- Ajout de la version de programme dans Vérification d'intégrité (Rapport)
* modGL_EJ.bas
- Ajout d'un .unprotect
* wshGL_EJ.doccls
- Ajout d'un .unprotect et d.un .protect
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_File_Usage.xlsx
+++ b/DataFiles/GCF_File_Usage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29286260-B123-4ED5-AA3F-63DA633282C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9623BC54-D9CA-46B5-990A-EAC67BBE6021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C6563B4-B351-4CD7-B6BC-9B6B7E0B5346}"/>
   </bookViews>
@@ -484,7 +484,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B3F5A5B-0475-4A13-A512-AE71167667D2}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
@@ -1766,6 +1766,53 @@
         <v>4892</v>
       </c>
     </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>45735.186921296299</v>
+      </c>
+      <c r="B28" s="3">
+        <v>10</v>
+      </c>
+      <c r="C28" s="3">
+        <v>6</v>
+      </c>
+      <c r="D28" s="3">
+        <v>249</v>
+      </c>
+      <c r="E28" s="3">
+        <v>452</v>
+      </c>
+      <c r="F28" s="3">
+        <v>428</v>
+      </c>
+      <c r="G28" s="3">
+        <v>478</v>
+      </c>
+      <c r="H28" s="3">
+        <v>3437</v>
+      </c>
+      <c r="I28" s="3">
+        <v>478</v>
+      </c>
+      <c r="J28" s="3">
+        <v>2026</v>
+      </c>
+      <c r="K28" s="3">
+        <v>208</v>
+      </c>
+      <c r="L28" s="3">
+        <v>418</v>
+      </c>
+      <c r="M28" s="3">
+        <v>30</v>
+      </c>
+      <c r="N28" s="3">
+        <v>3799</v>
+      </c>
+      <c r="O28" s="3">
+        <v>4968</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2025-03-25 @ 12:51 - Before comparaison
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_File_Usage.xlsx
+++ b/DataFiles/GCF_File_Usage.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9623BC54-D9CA-46B5-990A-EAC67BBE6021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA50E798-3F22-4C25-8159-6805B6D5660B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C6563B4-B351-4CD7-B6BC-9B6B7E0B5346}"/>
   </bookViews>
@@ -484,7 +484,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B3F5A5B-0475-4A13-A512-AE71167667D2}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
@@ -1813,6 +1813,194 @@
         <v>4968</v>
       </c>
     </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>45736.187303240738</v>
+      </c>
+      <c r="B29" s="3">
+        <v>10</v>
+      </c>
+      <c r="C29" s="3">
+        <v>6</v>
+      </c>
+      <c r="D29" s="3">
+        <v>265</v>
+      </c>
+      <c r="E29" s="3">
+        <v>453</v>
+      </c>
+      <c r="F29" s="3">
+        <v>429</v>
+      </c>
+      <c r="G29" s="3">
+        <v>478</v>
+      </c>
+      <c r="H29" s="3">
+        <v>3437</v>
+      </c>
+      <c r="I29" s="3">
+        <v>478</v>
+      </c>
+      <c r="J29" s="3">
+        <v>2026</v>
+      </c>
+      <c r="K29" s="3">
+        <v>208</v>
+      </c>
+      <c r="L29" s="3">
+        <v>418</v>
+      </c>
+      <c r="M29" s="3">
+        <v>30</v>
+      </c>
+      <c r="N29" s="3">
+        <v>3885</v>
+      </c>
+      <c r="O29" s="3">
+        <v>5002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>45737.18372685185</v>
+      </c>
+      <c r="B30" s="3">
+        <v>10</v>
+      </c>
+      <c r="C30" s="3">
+        <v>6</v>
+      </c>
+      <c r="D30" s="3">
+        <v>279</v>
+      </c>
+      <c r="E30" s="3">
+        <v>453</v>
+      </c>
+      <c r="F30" s="3">
+        <v>429</v>
+      </c>
+      <c r="G30" s="3">
+        <v>478</v>
+      </c>
+      <c r="H30" s="3">
+        <v>3437</v>
+      </c>
+      <c r="I30" s="3">
+        <v>478</v>
+      </c>
+      <c r="J30" s="3">
+        <v>2026</v>
+      </c>
+      <c r="K30" s="3">
+        <v>208</v>
+      </c>
+      <c r="L30" s="3">
+        <v>418</v>
+      </c>
+      <c r="M30" s="3">
+        <v>30</v>
+      </c>
+      <c r="N30" s="3">
+        <v>3935</v>
+      </c>
+      <c r="O30" s="3">
+        <v>5042</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>45737.189606481479</v>
+      </c>
+      <c r="B31" s="3">
+        <v>10</v>
+      </c>
+      <c r="C31" s="3">
+        <v>6</v>
+      </c>
+      <c r="D31" s="3">
+        <v>279</v>
+      </c>
+      <c r="E31" s="3">
+        <v>453</v>
+      </c>
+      <c r="F31" s="3">
+        <v>429</v>
+      </c>
+      <c r="G31" s="3">
+        <v>478</v>
+      </c>
+      <c r="H31" s="3">
+        <v>3437</v>
+      </c>
+      <c r="I31" s="3">
+        <v>478</v>
+      </c>
+      <c r="J31" s="3">
+        <v>2026</v>
+      </c>
+      <c r="K31" s="3">
+        <v>208</v>
+      </c>
+      <c r="L31" s="3">
+        <v>418</v>
+      </c>
+      <c r="M31" s="3">
+        <v>30</v>
+      </c>
+      <c r="N31" s="3">
+        <v>3935</v>
+      </c>
+      <c r="O31" s="3">
+        <v>5042</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>45738.185208333336</v>
+      </c>
+      <c r="B32" s="3">
+        <v>10</v>
+      </c>
+      <c r="C32" s="3">
+        <v>6</v>
+      </c>
+      <c r="D32" s="3">
+        <v>280</v>
+      </c>
+      <c r="E32" s="3">
+        <v>454</v>
+      </c>
+      <c r="F32" s="3">
+        <v>430</v>
+      </c>
+      <c r="G32" s="3">
+        <v>478</v>
+      </c>
+      <c r="H32" s="3">
+        <v>3437</v>
+      </c>
+      <c r="I32" s="3">
+        <v>478</v>
+      </c>
+      <c r="J32" s="3">
+        <v>2026</v>
+      </c>
+      <c r="K32" s="3">
+        <v>208</v>
+      </c>
+      <c r="L32" s="3">
+        <v>418</v>
+      </c>
+      <c r="M32" s="3">
+        <v>30</v>
+      </c>
+      <c r="N32" s="3">
+        <v>3941</v>
+      </c>
+      <c r="O32" s="3">
+        <v>5064</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2025-04-03 @ 05:47 - v6.C.4 - 29 475 lignes - Compile OK
* Casse
- GL ---> gl
- .ListBox ---> .listBox
- .selectedItems ---> .SelectedItems
* modDEV_Debug.bas
- Nouveau module
- Nouvelle procédure pour identifier les écarts entre les comptes clients (encaissements, facturation & grand livre)
* modDev_Proof.bas
 - Éliminer du code en commentaires (AnalyserFichiersLogSaisieHeures, AnalyserDossier, FnStripLigneLogSaisieHeures)
* modDev_Tools.bas
- Nouvelle procédure pour comparer 2 versions d'un classeur pour identifier les changements entre les 2 versions au niveau des cellules
* modENC_Saisie.bas
- Ajout de code pour confirmer que l'utilisateur veut quitter SANS mettre à jour l'encaissement à l'écran
* modImport.bas
- Ajout de code dans la procédure qu iimporte les transactions du Grand-livre en utilisant l'objet table
* modTEC_Evaluation.bas
- Mettre en commantaires un Debug.print
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_File_Usage.xlsx
+++ b/DataFiles/GCF_File_Usage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA50E798-3F22-4C25-8159-6805B6D5660B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68B3BF4-0639-4011-97CB-EB2BBE09D896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C6563B4-B351-4CD7-B6BC-9B6B7E0B5346}"/>
   </bookViews>
@@ -484,7 +484,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B3F5A5B-0475-4A13-A512-AE71167667D2}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
@@ -2001,6 +2001,335 @@
         <v>5064</v>
       </c>
     </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>45742.222743055558</v>
+      </c>
+      <c r="B33" s="3">
+        <v>10</v>
+      </c>
+      <c r="C33" s="3">
+        <v>6</v>
+      </c>
+      <c r="D33" s="3">
+        <v>280</v>
+      </c>
+      <c r="E33" s="3">
+        <v>454</v>
+      </c>
+      <c r="F33" s="3">
+        <v>430</v>
+      </c>
+      <c r="G33" s="3">
+        <v>478</v>
+      </c>
+      <c r="H33" s="3">
+        <v>3437</v>
+      </c>
+      <c r="I33" s="3">
+        <v>478</v>
+      </c>
+      <c r="J33" s="3">
+        <v>2026</v>
+      </c>
+      <c r="K33" s="3">
+        <v>208</v>
+      </c>
+      <c r="L33" s="3">
+        <v>418</v>
+      </c>
+      <c r="M33" s="3">
+        <v>30</v>
+      </c>
+      <c r="N33" s="3">
+        <v>3941</v>
+      </c>
+      <c r="O33" s="3">
+        <v>5180</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>45745.18310185185</v>
+      </c>
+      <c r="B34" s="3">
+        <v>10</v>
+      </c>
+      <c r="C34" s="3">
+        <v>6</v>
+      </c>
+      <c r="D34" s="3">
+        <v>286</v>
+      </c>
+      <c r="E34" s="3">
+        <v>466</v>
+      </c>
+      <c r="F34" s="3">
+        <v>441</v>
+      </c>
+      <c r="G34" s="3">
+        <v>478</v>
+      </c>
+      <c r="H34" s="3">
+        <v>3437</v>
+      </c>
+      <c r="I34" s="3">
+        <v>478</v>
+      </c>
+      <c r="J34" s="3">
+        <v>2026</v>
+      </c>
+      <c r="K34" s="3">
+        <v>208</v>
+      </c>
+      <c r="L34" s="3">
+        <v>418</v>
+      </c>
+      <c r="M34" s="3">
+        <v>30</v>
+      </c>
+      <c r="N34" s="3">
+        <v>3991</v>
+      </c>
+      <c r="O34" s="3">
+        <v>5286</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>45745.185428240744</v>
+      </c>
+      <c r="B35" s="3">
+        <v>10</v>
+      </c>
+      <c r="C35" s="3">
+        <v>6</v>
+      </c>
+      <c r="D35" s="3">
+        <v>286</v>
+      </c>
+      <c r="E35" s="3">
+        <v>466</v>
+      </c>
+      <c r="F35" s="3">
+        <v>441</v>
+      </c>
+      <c r="G35" s="3">
+        <v>478</v>
+      </c>
+      <c r="H35" s="3">
+        <v>3437</v>
+      </c>
+      <c r="I35" s="3">
+        <v>478</v>
+      </c>
+      <c r="J35" s="3">
+        <v>2026</v>
+      </c>
+      <c r="K35" s="3">
+        <v>208</v>
+      </c>
+      <c r="L35" s="3">
+        <v>418</v>
+      </c>
+      <c r="M35" s="3">
+        <v>30</v>
+      </c>
+      <c r="N35" s="3">
+        <v>3991</v>
+      </c>
+      <c r="O35" s="3">
+        <v>5286</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>45749.147685185184</v>
+      </c>
+      <c r="B36" s="3">
+        <v>10</v>
+      </c>
+      <c r="C36" s="3">
+        <v>6</v>
+      </c>
+      <c r="D36" s="3">
+        <v>299</v>
+      </c>
+      <c r="E36" s="3">
+        <v>474</v>
+      </c>
+      <c r="F36" s="3">
+        <v>449</v>
+      </c>
+      <c r="G36" s="3">
+        <v>534</v>
+      </c>
+      <c r="H36" s="3">
+        <v>4036</v>
+      </c>
+      <c r="I36" s="3">
+        <v>534</v>
+      </c>
+      <c r="J36" s="3">
+        <v>2556</v>
+      </c>
+      <c r="K36" s="3">
+        <v>255</v>
+      </c>
+      <c r="L36" s="3">
+        <v>494</v>
+      </c>
+      <c r="M36" s="3">
+        <v>30</v>
+      </c>
+      <c r="N36" s="3">
+        <v>4310</v>
+      </c>
+      <c r="O36" s="3">
+        <v>5373</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>45749.251122685186</v>
+      </c>
+      <c r="B37" s="3">
+        <v>10</v>
+      </c>
+      <c r="C37" s="3">
+        <v>6</v>
+      </c>
+      <c r="D37" s="3">
+        <v>299</v>
+      </c>
+      <c r="E37" s="3">
+        <v>474</v>
+      </c>
+      <c r="F37" s="3">
+        <v>449</v>
+      </c>
+      <c r="G37" s="3">
+        <v>534</v>
+      </c>
+      <c r="H37" s="3">
+        <v>4036</v>
+      </c>
+      <c r="I37" s="3">
+        <v>534</v>
+      </c>
+      <c r="J37" s="3">
+        <v>2556</v>
+      </c>
+      <c r="K37" s="3">
+        <v>255</v>
+      </c>
+      <c r="L37" s="3">
+        <v>494</v>
+      </c>
+      <c r="M37" s="3">
+        <v>30</v>
+      </c>
+      <c r="N37" s="3">
+        <v>4310</v>
+      </c>
+      <c r="O37" s="3">
+        <v>5373</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <v>45749.331574074073</v>
+      </c>
+      <c r="B38" s="3">
+        <v>10</v>
+      </c>
+      <c r="C38" s="3">
+        <v>6</v>
+      </c>
+      <c r="D38" s="3">
+        <v>299</v>
+      </c>
+      <c r="E38" s="3">
+        <v>474</v>
+      </c>
+      <c r="F38" s="3">
+        <v>449</v>
+      </c>
+      <c r="G38" s="3">
+        <v>534</v>
+      </c>
+      <c r="H38" s="3">
+        <v>4036</v>
+      </c>
+      <c r="I38" s="3">
+        <v>534</v>
+      </c>
+      <c r="J38" s="3">
+        <v>2556</v>
+      </c>
+      <c r="K38" s="3">
+        <v>255</v>
+      </c>
+      <c r="L38" s="3">
+        <v>494</v>
+      </c>
+      <c r="M38" s="3">
+        <v>30</v>
+      </c>
+      <c r="N38" s="3">
+        <v>4314</v>
+      </c>
+      <c r="O38" s="3">
+        <v>5373</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
+        <v>45750.121944444443</v>
+      </c>
+      <c r="B39" s="3">
+        <v>10</v>
+      </c>
+      <c r="C39" s="3">
+        <v>6</v>
+      </c>
+      <c r="D39" s="3">
+        <v>299</v>
+      </c>
+      <c r="E39" s="3">
+        <v>474</v>
+      </c>
+      <c r="F39" s="3">
+        <v>449</v>
+      </c>
+      <c r="G39" s="3">
+        <v>534</v>
+      </c>
+      <c r="H39" s="3">
+        <v>4036</v>
+      </c>
+      <c r="I39" s="3">
+        <v>534</v>
+      </c>
+      <c r="J39" s="3">
+        <v>2570</v>
+      </c>
+      <c r="K39" s="3">
+        <v>257</v>
+      </c>
+      <c r="L39" s="3">
+        <v>494</v>
+      </c>
+      <c r="M39" s="3">
+        <v>30</v>
+      </c>
+      <c r="N39" s="3">
+        <v>4314</v>
+      </c>
+      <c r="O39" s="3">
+        <v>5402</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2025-05-02 @ 14:09 - Clients_v5.7.xlsm - 1 698 lignes - Compile OK
* Ajout de l'ouverture de EXCEL pour forcer l'écriture incertaine avec ADO ???
* modMain.bas
- Code pour ouvrir temporairement EXCEL pour forcer l'écriture
- Ajout de la date dans le log pour analyser la date de la dernière modification
* modUtils.bas
- Ajout de la date dans le log pour analyser la date de la dernière modification
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_File_Usage.xlsx
+++ b/DataFiles/GCF_File_Usage.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68B3BF4-0639-4011-97CB-EB2BBE09D896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B08BC3-2E85-4988-8FD0-5D9C5E95C08C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C6563B4-B351-4CD7-B6BC-9B6B7E0B5346}"/>
   </bookViews>
@@ -484,7 +484,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B3F5A5B-0475-4A13-A512-AE71167667D2}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:O39"/>
+  <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
@@ -2330,6 +2330,53 @@
         <v>5402</v>
       </c>
     </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
+        <v>45779.4450462963</v>
+      </c>
+      <c r="B40" s="3">
+        <v>10</v>
+      </c>
+      <c r="C40" s="3">
+        <v>6</v>
+      </c>
+      <c r="D40" s="3">
+        <v>299</v>
+      </c>
+      <c r="E40" s="3">
+        <v>474</v>
+      </c>
+      <c r="F40" s="3">
+        <v>449</v>
+      </c>
+      <c r="G40" s="3">
+        <v>534</v>
+      </c>
+      <c r="H40" s="3">
+        <v>4036</v>
+      </c>
+      <c r="I40" s="3">
+        <v>534</v>
+      </c>
+      <c r="J40" s="3">
+        <v>2570</v>
+      </c>
+      <c r="K40" s="3">
+        <v>257</v>
+      </c>
+      <c r="L40" s="3">
+        <v>494</v>
+      </c>
+      <c r="M40" s="3">
+        <v>30</v>
+      </c>
+      <c r="N40" s="3">
+        <v>4314</v>
+      </c>
+      <c r="O40" s="3">
+        <v>5402</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2025-05-06 @ 11:38 - v6.C.4.1.xlsb - 29 612 lignes - Compile OK
* modFAC_Finale.bas
- Modifications à la procédure 'FAC_Finale_Creation_PDF' pour stabiliser/sécuriser le traitement
- Changer l'approche de la copie de l'entête vers le fichier Excel du client
* modFunctions.bas
- Ajouter des fonctions TRIM pour la recherche des noms de clients
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_File_Usage.xlsx
+++ b/DataFiles/GCF_File_Usage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B08BC3-2E85-4988-8FD0-5D9C5E95C08C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77193E5E-1DD5-47DA-9111-BEFFC287692C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C6563B4-B351-4CD7-B6BC-9B6B7E0B5346}"/>
   </bookViews>
@@ -484,7 +484,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B3F5A5B-0475-4A13-A512-AE71167667D2}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:O40"/>
+  <dimension ref="A1:O44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
@@ -2377,6 +2377,194 @@
         <v>5402</v>
       </c>
     </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="5">
+        <v>45779.894999999997</v>
+      </c>
+      <c r="B41" s="3">
+        <v>10</v>
+      </c>
+      <c r="C41" s="3">
+        <v>6</v>
+      </c>
+      <c r="D41" s="3">
+        <v>360</v>
+      </c>
+      <c r="E41" s="3">
+        <v>537</v>
+      </c>
+      <c r="F41" s="3">
+        <v>512</v>
+      </c>
+      <c r="G41" s="3">
+        <v>565</v>
+      </c>
+      <c r="H41" s="3">
+        <v>4214</v>
+      </c>
+      <c r="I41" s="3">
+        <v>565</v>
+      </c>
+      <c r="J41" s="3">
+        <v>2728</v>
+      </c>
+      <c r="K41" s="3">
+        <v>268</v>
+      </c>
+      <c r="L41" s="3">
+        <v>510</v>
+      </c>
+      <c r="M41" s="3">
+        <v>30</v>
+      </c>
+      <c r="N41" s="3">
+        <v>4843</v>
+      </c>
+      <c r="O41" s="3">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="5">
+        <v>45782.992569444446</v>
+      </c>
+      <c r="B42" s="3">
+        <v>10</v>
+      </c>
+      <c r="C42" s="3">
+        <v>6</v>
+      </c>
+      <c r="D42" s="3">
+        <v>360</v>
+      </c>
+      <c r="E42" s="3">
+        <v>538</v>
+      </c>
+      <c r="F42" s="3">
+        <v>513</v>
+      </c>
+      <c r="G42" s="3">
+        <v>572</v>
+      </c>
+      <c r="H42" s="3">
+        <v>4292</v>
+      </c>
+      <c r="I42" s="3">
+        <v>572</v>
+      </c>
+      <c r="J42" s="3">
+        <v>2842</v>
+      </c>
+      <c r="K42" s="3">
+        <v>278</v>
+      </c>
+      <c r="L42" s="3">
+        <v>519</v>
+      </c>
+      <c r="M42" s="3">
+        <v>30</v>
+      </c>
+      <c r="N42" s="3">
+        <v>4875</v>
+      </c>
+      <c r="O42" s="3">
+        <v>6448</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="5">
+        <v>45783.482037037036</v>
+      </c>
+      <c r="B43" s="3">
+        <v>10</v>
+      </c>
+      <c r="C43" s="3">
+        <v>6</v>
+      </c>
+      <c r="D43" s="3">
+        <v>360</v>
+      </c>
+      <c r="E43" s="3">
+        <v>538</v>
+      </c>
+      <c r="F43" s="3">
+        <v>513</v>
+      </c>
+      <c r="G43" s="3">
+        <v>577</v>
+      </c>
+      <c r="H43" s="3">
+        <v>4305</v>
+      </c>
+      <c r="I43" s="3">
+        <v>577</v>
+      </c>
+      <c r="J43" s="3">
+        <v>3084</v>
+      </c>
+      <c r="K43" s="3">
+        <v>284</v>
+      </c>
+      <c r="L43" s="3">
+        <v>527</v>
+      </c>
+      <c r="M43" s="3">
+        <v>30</v>
+      </c>
+      <c r="N43" s="3">
+        <v>4875</v>
+      </c>
+      <c r="O43" s="3">
+        <v>6448</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="5">
+        <v>45783.483414351853</v>
+      </c>
+      <c r="B44" s="3">
+        <v>10</v>
+      </c>
+      <c r="C44" s="3">
+        <v>6</v>
+      </c>
+      <c r="D44" s="3">
+        <v>360</v>
+      </c>
+      <c r="E44" s="3">
+        <v>538</v>
+      </c>
+      <c r="F44" s="3">
+        <v>513</v>
+      </c>
+      <c r="G44" s="3">
+        <v>577</v>
+      </c>
+      <c r="H44" s="3">
+        <v>4305</v>
+      </c>
+      <c r="I44" s="3">
+        <v>577</v>
+      </c>
+      <c r="J44" s="3">
+        <v>3084</v>
+      </c>
+      <c r="K44" s="3">
+        <v>284</v>
+      </c>
+      <c r="L44" s="3">
+        <v>527</v>
+      </c>
+      <c r="M44" s="3">
+        <v>30</v>
+      </c>
+      <c r="N44" s="3">
+        <v>4920</v>
+      </c>
+      <c r="O44" s="3">
+        <v>6448</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2025-05-06 @ 23:00 - v6.C.4.2.xlsb - 29 602 lignes - Compile OK
* modDEB_Saisie.bas
- Modifications pour le code de taxe 'M'
* modTEC_Saisie.bas
- Ajout de code pour tenter de déboguer l'activation des boutons
* ufSaisieHeures.frm
- Ajout de code pour tenter de déboguer l'activation des boutons
* wshDEB_Saisie.doccls
- Mise en commentaire un test sur le code de taxe 'M'
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_File_Usage.xlsx
+++ b/DataFiles/GCF_File_Usage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77193E5E-1DD5-47DA-9111-BEFFC287692C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF072BCF-5BC0-4374-9131-044C481FD4C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C6563B4-B351-4CD7-B6BC-9B6B7E0B5346}"/>
   </bookViews>
@@ -484,7 +484,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B3F5A5B-0475-4A13-A512-AE71167667D2}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:O44"/>
+  <dimension ref="A1:O46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
@@ -2565,6 +2565,100 @@
         <v>6448</v>
       </c>
     </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="5">
+        <v>45783.953576388885</v>
+      </c>
+      <c r="B45" s="3">
+        <v>10</v>
+      </c>
+      <c r="C45" s="3">
+        <v>6</v>
+      </c>
+      <c r="D45" s="3">
+        <v>365</v>
+      </c>
+      <c r="E45" s="3">
+        <v>539</v>
+      </c>
+      <c r="F45" s="3">
+        <v>514</v>
+      </c>
+      <c r="G45" s="3">
+        <v>572</v>
+      </c>
+      <c r="H45" s="3">
+        <v>4292</v>
+      </c>
+      <c r="I45" s="3">
+        <v>572</v>
+      </c>
+      <c r="J45" s="3">
+        <v>2842</v>
+      </c>
+      <c r="K45" s="3">
+        <v>278</v>
+      </c>
+      <c r="L45" s="3">
+        <v>519</v>
+      </c>
+      <c r="M45" s="3">
+        <v>30</v>
+      </c>
+      <c r="N45" s="3">
+        <v>4903</v>
+      </c>
+      <c r="O45" s="3">
+        <v>6479</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="5">
+        <v>45783.95579861111</v>
+      </c>
+      <c r="B46" s="3">
+        <v>10</v>
+      </c>
+      <c r="C46" s="3">
+        <v>6</v>
+      </c>
+      <c r="D46" s="3">
+        <v>365</v>
+      </c>
+      <c r="E46" s="3">
+        <v>539</v>
+      </c>
+      <c r="F46" s="3">
+        <v>514</v>
+      </c>
+      <c r="G46" s="3">
+        <v>572</v>
+      </c>
+      <c r="H46" s="3">
+        <v>4292</v>
+      </c>
+      <c r="I46" s="3">
+        <v>572</v>
+      </c>
+      <c r="J46" s="3">
+        <v>2841</v>
+      </c>
+      <c r="K46" s="3">
+        <v>277</v>
+      </c>
+      <c r="L46" s="3">
+        <v>519</v>
+      </c>
+      <c r="M46" s="3">
+        <v>30</v>
+      </c>
+      <c r="N46" s="3">
+        <v>4903</v>
+      </c>
+      <c r="O46" s="3">
+        <v>6479</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2025-09-26 @ 10:46 - v6.C.6.xlsb - 28 404 lignes - Compile OK
* modImport.bas
- Changer le nom de la colonne (26 ---> Z)
* wshTEC_Analyse.doccls
- Enlever les lignes en commentaires
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_File_Usage.xlsx
+++ b/DataFiles/GCF_File_Usage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F4B3D8-709C-4DEF-8D07-5B5C06E52529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D1C06EE-CD10-4FC1-B115-89A5E13C1B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C6563B4-B351-4CD7-B6BC-9B6B7E0B5346}"/>
   </bookViews>
@@ -484,7 +484,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B3F5A5B-0475-4A13-A512-AE71167667D2}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:O65"/>
+  <dimension ref="A1:O73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
@@ -3552,6 +3552,382 @@
         <v>6551</v>
       </c>
     </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A66" s="5">
+        <v>45791.341157407405</v>
+      </c>
+      <c r="B66" s="3">
+        <v>11</v>
+      </c>
+      <c r="C66" s="3">
+        <v>6</v>
+      </c>
+      <c r="D66" s="3">
+        <v>366</v>
+      </c>
+      <c r="E66" s="3">
+        <v>545</v>
+      </c>
+      <c r="F66" s="3">
+        <v>518</v>
+      </c>
+      <c r="G66" s="3">
+        <v>575</v>
+      </c>
+      <c r="H66" s="3">
+        <v>4305</v>
+      </c>
+      <c r="I66" s="3">
+        <v>575</v>
+      </c>
+      <c r="J66" s="3">
+        <v>2841</v>
+      </c>
+      <c r="K66" s="3">
+        <v>277</v>
+      </c>
+      <c r="L66" s="3">
+        <v>519</v>
+      </c>
+      <c r="M66" s="3">
+        <v>30</v>
+      </c>
+      <c r="N66" s="3">
+        <v>4919</v>
+      </c>
+      <c r="O66" s="3">
+        <v>6551</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A67" s="5">
+        <v>45791.348599537036</v>
+      </c>
+      <c r="B67" s="3">
+        <v>11</v>
+      </c>
+      <c r="C67" s="3">
+        <v>6</v>
+      </c>
+      <c r="D67" s="3">
+        <v>366</v>
+      </c>
+      <c r="E67" s="3">
+        <v>545</v>
+      </c>
+      <c r="F67" s="3">
+        <v>518</v>
+      </c>
+      <c r="G67" s="3">
+        <v>575</v>
+      </c>
+      <c r="H67" s="3">
+        <v>4305</v>
+      </c>
+      <c r="I67" s="3">
+        <v>575</v>
+      </c>
+      <c r="J67" s="3">
+        <v>2841</v>
+      </c>
+      <c r="K67" s="3">
+        <v>277</v>
+      </c>
+      <c r="L67" s="3">
+        <v>519</v>
+      </c>
+      <c r="M67" s="3">
+        <v>30</v>
+      </c>
+      <c r="N67" s="3">
+        <v>4919</v>
+      </c>
+      <c r="O67" s="3">
+        <v>6551</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A68" s="5">
+        <v>45792.00105324074</v>
+      </c>
+      <c r="B68" s="3">
+        <v>11</v>
+      </c>
+      <c r="C68" s="3">
+        <v>6</v>
+      </c>
+      <c r="D68" s="3">
+        <v>375</v>
+      </c>
+      <c r="E68" s="3">
+        <v>558</v>
+      </c>
+      <c r="F68" s="3">
+        <v>531</v>
+      </c>
+      <c r="G68" s="3">
+        <v>575</v>
+      </c>
+      <c r="H68" s="3">
+        <v>4305</v>
+      </c>
+      <c r="I68" s="3">
+        <v>575</v>
+      </c>
+      <c r="J68" s="3">
+        <v>2841</v>
+      </c>
+      <c r="K68" s="3">
+        <v>277</v>
+      </c>
+      <c r="L68" s="3">
+        <v>519</v>
+      </c>
+      <c r="M68" s="3">
+        <v>30</v>
+      </c>
+      <c r="N68" s="3">
+        <v>5032</v>
+      </c>
+      <c r="O68" s="3">
+        <v>6630</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A69" s="5">
+        <v>45795.334745370368</v>
+      </c>
+      <c r="B69" s="3">
+        <v>11</v>
+      </c>
+      <c r="C69" s="3">
+        <v>6</v>
+      </c>
+      <c r="D69" s="3">
+        <v>379</v>
+      </c>
+      <c r="E69" s="3">
+        <v>558</v>
+      </c>
+      <c r="F69" s="3">
+        <v>531</v>
+      </c>
+      <c r="G69" s="3">
+        <v>620</v>
+      </c>
+      <c r="H69" s="3">
+        <v>4751</v>
+      </c>
+      <c r="I69" s="3">
+        <v>620</v>
+      </c>
+      <c r="J69" s="3">
+        <v>3881</v>
+      </c>
+      <c r="K69" s="3">
+        <v>369</v>
+      </c>
+      <c r="L69" s="3">
+        <v>580</v>
+      </c>
+      <c r="M69" s="3">
+        <v>30</v>
+      </c>
+      <c r="N69" s="3">
+        <v>5221</v>
+      </c>
+      <c r="O69" s="3">
+        <v>6695</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A70" s="5">
+        <v>45795.86577546296</v>
+      </c>
+      <c r="B70" s="3">
+        <v>11</v>
+      </c>
+      <c r="C70" s="3">
+        <v>6</v>
+      </c>
+      <c r="D70" s="3">
+        <v>379</v>
+      </c>
+      <c r="E70" s="3">
+        <v>558</v>
+      </c>
+      <c r="F70" s="3">
+        <v>531</v>
+      </c>
+      <c r="G70" s="3">
+        <v>671</v>
+      </c>
+      <c r="H70" s="3">
+        <v>5349</v>
+      </c>
+      <c r="I70" s="3">
+        <v>671</v>
+      </c>
+      <c r="J70" s="3">
+        <v>672</v>
+      </c>
+      <c r="K70" s="3">
+        <v>49</v>
+      </c>
+      <c r="L70" s="3">
+        <v>655</v>
+      </c>
+      <c r="M70" s="3">
+        <v>30</v>
+      </c>
+      <c r="N70" s="3">
+        <v>5466</v>
+      </c>
+      <c r="O70" s="3">
+        <v>6701</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A71" s="5">
+        <v>45799.25136574074</v>
+      </c>
+      <c r="B71" s="3">
+        <v>11</v>
+      </c>
+      <c r="C71" s="3">
+        <v>6</v>
+      </c>
+      <c r="D71" s="3">
+        <v>383</v>
+      </c>
+      <c r="E71" s="3">
+        <v>579</v>
+      </c>
+      <c r="F71" s="3">
+        <v>552</v>
+      </c>
+      <c r="G71" s="3">
+        <v>673</v>
+      </c>
+      <c r="H71" s="3">
+        <v>5361</v>
+      </c>
+      <c r="I71" s="3">
+        <v>673</v>
+      </c>
+      <c r="J71" s="3">
+        <v>50</v>
+      </c>
+      <c r="K71" s="3">
+        <v>4</v>
+      </c>
+      <c r="L71" s="3">
+        <v>656</v>
+      </c>
+      <c r="M71" s="3">
+        <v>30</v>
+      </c>
+      <c r="N71" s="3">
+        <v>5530</v>
+      </c>
+      <c r="O71" s="3">
+        <v>6775</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A72" s="5">
+        <v>45799.260034722225</v>
+      </c>
+      <c r="B72" s="3">
+        <v>11</v>
+      </c>
+      <c r="C72" s="3">
+        <v>6</v>
+      </c>
+      <c r="D72" s="3">
+        <v>383</v>
+      </c>
+      <c r="E72" s="3">
+        <v>579</v>
+      </c>
+      <c r="F72" s="3">
+        <v>552</v>
+      </c>
+      <c r="G72" s="3">
+        <v>673</v>
+      </c>
+      <c r="H72" s="3">
+        <v>5361</v>
+      </c>
+      <c r="I72" s="3">
+        <v>673</v>
+      </c>
+      <c r="J72" s="3">
+        <v>50</v>
+      </c>
+      <c r="K72" s="3">
+        <v>4</v>
+      </c>
+      <c r="L72" s="3">
+        <v>656</v>
+      </c>
+      <c r="M72" s="3">
+        <v>30</v>
+      </c>
+      <c r="N72" s="3">
+        <v>5530</v>
+      </c>
+      <c r="O72" s="3">
+        <v>6775</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A73" s="5">
+        <v>45802.923344907409</v>
+      </c>
+      <c r="B73" s="3">
+        <v>11</v>
+      </c>
+      <c r="C73" s="3">
+        <v>6</v>
+      </c>
+      <c r="D73" s="3">
+        <v>385</v>
+      </c>
+      <c r="E73" s="3">
+        <v>606</v>
+      </c>
+      <c r="F73" s="3">
+        <v>578</v>
+      </c>
+      <c r="G73" s="3">
+        <v>682</v>
+      </c>
+      <c r="H73" s="3">
+        <v>5472</v>
+      </c>
+      <c r="I73" s="3">
+        <v>682</v>
+      </c>
+      <c r="J73" s="3">
+        <v>237</v>
+      </c>
+      <c r="K73" s="3">
+        <v>12</v>
+      </c>
+      <c r="L73" s="3">
+        <v>673</v>
+      </c>
+      <c r="M73" s="3">
+        <v>30</v>
+      </c>
+      <c r="N73" s="3">
+        <v>5635</v>
+      </c>
+      <c r="O73" s="3">
+        <v>6845</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2025-06-11 @ 10:36 - v6.C.94.xlsb - 30 256 lignes - Compile OK
* ufSaisieHeures.frm
- Ne plus utiliser la procédure 'ActiverButtonsVraiOuFaux' pour déterminer quels boutons doivent être Actifs ou Inactifs
- Effacer les lignes en 'CommentOut'
- Ajout d'une procédure 'VerifierEtatBoutonAjouter ' pour déterminer si le bouton AJOUTER doit être Actif ou Inactif
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_File_Usage.xlsx
+++ b/DataFiles/GCF_File_Usage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8728EFF8-6D4E-4ED5-9B26-C2A33B03BF30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB419C6-3F23-4819-962E-85A767144C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C6563B4-B351-4CD7-B6BC-9B6B7E0B5346}"/>
   </bookViews>
@@ -484,7 +484,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B3F5A5B-0475-4A13-A512-AE71167667D2}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:O84"/>
+  <dimension ref="A1:O85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
@@ -4445,6 +4445,53 @@
         <v>7100</v>
       </c>
     </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A85" s="5">
+        <v>45816.677997685183</v>
+      </c>
+      <c r="B85" s="3">
+        <v>14</v>
+      </c>
+      <c r="C85" s="3">
+        <v>6</v>
+      </c>
+      <c r="D85" s="3">
+        <v>414</v>
+      </c>
+      <c r="E85" s="3">
+        <v>650</v>
+      </c>
+      <c r="F85" s="3">
+        <v>622</v>
+      </c>
+      <c r="G85" s="3">
+        <v>692</v>
+      </c>
+      <c r="H85" s="3">
+        <v>5568</v>
+      </c>
+      <c r="I85" s="3">
+        <v>692</v>
+      </c>
+      <c r="J85" s="3">
+        <v>2</v>
+      </c>
+      <c r="K85" s="3">
+        <v>2</v>
+      </c>
+      <c r="L85" s="3">
+        <v>684</v>
+      </c>
+      <c r="M85" s="3">
+        <v>30</v>
+      </c>
+      <c r="N85" s="3">
+        <v>5916</v>
+      </c>
+      <c r="O85" s="3">
+        <v>7100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>